<commit_message>
updated notebooks for data analysis
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/Book4.xlsx
+++ b/REyeker-DataAnalyses-Python/Book4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arooba\Desktop\StudyData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\REyeker\REyeker-DataAnalyses-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC09AF-6DFB-47B1-82C8-098F2748BBE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="data_RecursiveIterative_2021-01-07_02-43" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="data_RecursiveIterative_2021-01-07_02-43" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\Arooba\Downloads\Assignment5\data_RecursiveIterative_2021-01-07_02-43.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="445">
         <textField/>
@@ -5381,9 +5382,6 @@
     <t>6 6 6 \n12 12 12 \n18 18 18 \n</t>
   </si>
   <si>
-    <t xml:space="preserve">168-44 325-19 260-51 88-47 409-45 551-67 275-82 133-82 130-107 128-121 120-167 128-200 385-187 59-227 122-258 245-271 57-314 180-287 172-272 200-264 177-228 188-101 166-38 146-91 201-98 147-200 145-248 172-282 209-282 165-210 179-266 223-202 230-267 142-234 155-281 180-271 252--1 173-69 255-278 86-7 212-77 206-277 199-89 216-274 209-206 163-250 198-274 146-112 137-62 97-87 106-92 166-202 400-182 216-240 100-220 138-248 135-275 192-271 115-274 160-272 236-207 293-125 422-184 138-200 159-231 169-255 170-12 188-84 233-218 207-235 209-131 167-95 205-79 200-237 153-295 157-280 307-325 399-311 322-306 177-279 178-238 247-195 223-256 258-275 351-327 315-296 175-257 129-272 205-266 165-214 423-177 211-225 81-221 136-241 138-208 137-257 126-229 137-210 122-217 132-265 161-294 171-275 205-242 209-268 176-207 176-225 176-225 180-205 276-194 489-210 158-235 126-275 131-272 162-82 173-266 180-121 182-98 181-80 189-287 148-258 168-89 166-255 173-279 168-280 169-265 163-275 177-309 199-275 267-224 278-277 </t>
-  </si>
-  <si>
     <t xml:space="preserve">136-77 99-28 289-28 289-28 581-75 208-66 297-70 466-91 121-107 332-80 248-141 360-122 206-141 97-161 339-157 197-181 593-194 128-276 285-245 206-211 121-292 378-341 519-334 541-332 201-358 448-375 249-358 83-372 268-417 146-399 462-434 386-389 199-427 217-418 210-421 225-468 227-518 212-549 192-612 166-554 259-395 247-357 232-454 196-415 608-326 187-420 192-378 456-415 267-430 422-415 148-414 345-400 236-410 306-405 178-461 161-492 283-577 173-578 221-452 233-389 223-522 246-555 230-601 235-584 202-495 207-437 220-388 285-409 232-400 408-416 243-429 117-449 222-448 190-445 325-89 340-81 207-504 189-465 166-447 215-396 206-380 239-480 246-402 220-438 227-486 226-444 226-460 226-486 229-557 196-600 187-632 200-555 210-516 367-65 283-421 238-480 197-530 220-514 233-422 215-522 346-102 341-74 196-552 179-522 180-474 213-436 192-370 219-480 190-468 316-164 320-117 318-281 296-378 112-657 186-547 170-474 153-431 223-378 162-351 262-390 139-378 218-378 232-398 161-411 221-406 223-455 159-414 168-439 171-524 149-577 175-640 256-91 188-400 168-354 221-359 340-338 459-347 199-369 169-390 173-368 171-397 201-412 188-397 235-406 221-441 165-467 182-492 228-370 199-411 335-407 201-414 287-409 220-444 262-425 199-499 170-518 198-498 219-515 181-527 221-524 236-392 197-439 246-397 290-410 235-476 239-555 197-537 193-516 173-516 398-381 356-397 269-407 241-419 232-408 316-418 372-414 118-406 266-386 159-408 225-396 367-405 208-401 222-408 200-435 325-159 337-84 221-486 365-462 337-282 336-98 </t>
   </si>
   <si>
@@ -5988,12 +5986,15 @@
   </si>
   <si>
     <t xml:space="preserve">331-118 298-56 284-76 144-20 166-93 155-256 215-84 235-117 437-127 320-108 237-85 185-268 181-346 186-404 193-469 235-219 221-275 203-323 307-352 248-388 240-440 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">168-44 325-19 260-51 88-47 409-45 551-67 275-82 133-82 130-107 128-121 120-167 128-200 385-187 59-227 122-258 245-271 57-314 180-287 172-272 200-264 177-228 188-101 166-38 146-91 201-98 147-200 145-248 172-282 209-282 165-210 179-266 223-202 230-267 142-234 155-281 180-271 252-1 173-69 255-278 86-7 212-77 206-277 199-89 216-274 209-206 163-250 198-274 146-112 137-62 97-87 106-92 166-202 400-182 216-240 100-220 138-248 135-275 192-271 115-274 160-272 236-207 293-125 422-184 138-200 159-231 169-255 170-12 188-84 233-218 207-235 209-131 167-95 205-79 200-237 153-295 157-280 307-325 399-311 322-306 177-279 178-238 247-195 223-256 258-275 351-327 315-296 175-257 129-272 205-266 165-214 423-177 211-225 81-221 136-241 138-208 137-257 126-229 137-210 122-217 132-265 161-294 171-275 205-242 209-268 176-207 176-225 176-225 180-205 276-194 489-210 158-235 126-275 131-272 162-82 173-266 180-121 182-98 181-80 189-287 148-258 168-89 166-255 173-279 168-280 169-265 163-275 177-309 199-275 267-224 278-277 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6030,7 +6031,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6046,7 +6047,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data_RecursiveIterative_2021-01-07_02-43" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data_RecursiveIterative_2021-01-07_02-43" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6311,355 +6312,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:QC193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="IA138" workbookViewId="0">
+      <selection activeCell="IG152" sqref="IG152"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="75.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="62.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="45" max="48" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="80.33203125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="86" max="90" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="41.5546875" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="127" max="131" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="72.88671875" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="148" max="149" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="157" max="158" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="68.88671875" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="168" max="171" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="62.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="48" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="80.28515625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="90" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="127" max="131" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="148" max="149" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="157" max="158" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="168" max="171" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="178" max="178" width="42" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="181" max="181" width="9" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="199" max="199" width="48" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="73.77734375" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="231" max="231" width="31" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="241" max="244" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="241" max="244" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="253" max="253" width="60" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="70.88671875" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="71.5546875" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="48.88671875" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="46.44140625" bestFit="1" customWidth="1"/>
-    <col min="281" max="284" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="287" max="287" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="288" max="288" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="289" max="289" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="292" max="292" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="52.88671875" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="299" max="299" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="300" max="300" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="301" max="301" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="62.109375" bestFit="1" customWidth="1"/>
-    <col min="303" max="303" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="304" max="304" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="305" max="305" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="310" max="310" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="311" max="311" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="315" max="315" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="316" max="316" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="320" max="325" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="326" max="326" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="328" max="328" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="329" max="329" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="330" max="330" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="331" max="331" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="332" max="332" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="333" max="333" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="334" max="334" width="52.33203125" bestFit="1" customWidth="1"/>
-    <col min="335" max="335" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="336" max="336" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="337" max="337" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="338" max="338" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="339" max="339" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="340" max="340" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="341" max="341" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="342" max="342" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="344" max="344" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="345" max="345" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="346" max="346" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="347" max="347" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="348" max="348" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="349" max="349" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="350" max="350" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="351" max="351" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="352" max="352" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="353" max="353" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="354" max="354" width="55.109375" bestFit="1" customWidth="1"/>
-    <col min="355" max="355" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="356" max="356" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="357" max="357" width="47.44140625" bestFit="1" customWidth="1"/>
-    <col min="358" max="358" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="359" max="359" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="360" max="363" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="364" max="372" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="373" max="438" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="281" max="284" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="287" max="287" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="288" max="288" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="289" max="289" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="290" max="290" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="292" max="292" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="295" max="295" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="296" max="296" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="297" max="297" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="299" max="299" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="300" max="300" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="301" max="301" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="62.140625" bestFit="1" customWidth="1"/>
+    <col min="303" max="303" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="304" max="304" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="305" max="305" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="309" max="309" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="310" max="310" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="311" max="311" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="312" max="312" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="313" max="313" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="314" max="314" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="315" max="315" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="316" max="316" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="317" max="317" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="320" max="325" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="326" max="326" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="327" max="327" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="328" max="328" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="329" max="329" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="330" max="330" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="331" max="331" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="332" max="332" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="333" max="333" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="334" max="334" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="335" max="335" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="336" max="336" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="337" max="337" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="338" max="338" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="339" max="339" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="340" max="340" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="341" max="341" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="342" max="342" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="343" max="343" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="344" max="344" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="345" max="345" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="346" max="346" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="347" max="347" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="348" max="348" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="349" max="349" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="350" max="350" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="351" max="351" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="352" max="352" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="353" max="353" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="354" max="354" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="355" max="355" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="356" max="356" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="357" max="357" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="358" max="358" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="359" max="359" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="360" max="363" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="364" max="372" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="373" max="438" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="439" max="439" width="30" bestFit="1" customWidth="1"/>
-    <col min="440" max="440" width="68.109375" bestFit="1" customWidth="1"/>
-    <col min="441" max="441" width="40.21875" bestFit="1" customWidth="1"/>
-    <col min="442" max="442" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="443" max="443" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="444" max="444" width="52.5546875" bestFit="1" customWidth="1"/>
-    <col min="445" max="445" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="440" max="440" width="68.140625" bestFit="1" customWidth="1"/>
+    <col min="441" max="441" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="442" max="442" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="443" max="443" width="66.28515625" bestFit="1" customWidth="1"/>
+    <col min="444" max="444" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="445" max="445" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7996,7 +7999,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="2" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>445</v>
       </c>
@@ -9333,7 +9336,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>620</v>
       </c>
@@ -9377,7 +9380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>621</v>
       </c>
@@ -9421,7 +9424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>622</v>
       </c>
@@ -9465,7 +9468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>623</v>
       </c>
@@ -9512,7 +9515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>630</v>
       </c>
@@ -9556,7 +9559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>631</v>
       </c>
@@ -9963,7 +9966,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>636</v>
       </c>
@@ -10040,7 +10043,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>637</v>
       </c>
@@ -10111,7 +10114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>638</v>
       </c>
@@ -10503,7 +10506,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>639</v>
       </c>
@@ -10550,7 +10553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>642</v>
       </c>
@@ -10594,7 +10597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>643</v>
       </c>
@@ -10866,7 +10869,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>644</v>
       </c>
@@ -10940,7 +10943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>645</v>
       </c>
@@ -10984,7 +10987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>653</v>
       </c>
@@ -11388,7 +11391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>659</v>
       </c>
@@ -11492,7 +11495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>660</v>
       </c>
@@ -11536,7 +11539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>661</v>
       </c>
@@ -11580,7 +11583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>663</v>
       </c>
@@ -11642,7 +11645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>693</v>
       </c>
@@ -11752,7 +11755,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>694</v>
       </c>
@@ -12150,7 +12153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>696</v>
       </c>
@@ -12428,7 +12431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>699</v>
       </c>
@@ -12823,7 +12826,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>700</v>
       </c>
@@ -13218,7 +13221,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>701</v>
       </c>
@@ -13292,7 +13295,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>702</v>
       </c>
@@ -13366,7 +13369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>703</v>
       </c>
@@ -13755,7 +13758,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>704</v>
       </c>
@@ -14153,7 +14156,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>705</v>
       </c>
@@ -14197,7 +14200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>706</v>
       </c>
@@ -14472,7 +14475,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>707</v>
       </c>
@@ -14753,7 +14756,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>708</v>
       </c>
@@ -15142,7 +15145,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>709</v>
       </c>
@@ -15546,7 +15549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>710</v>
       </c>
@@ -15608,7 +15611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>711</v>
       </c>
@@ -15958,7 +15961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>712</v>
       </c>
@@ -16353,7 +16356,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>713</v>
       </c>
@@ -16397,7 +16400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>714</v>
       </c>
@@ -16441,7 +16444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>715</v>
       </c>
@@ -16722,7 +16725,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>716</v>
       </c>
@@ -17000,7 +17003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>717</v>
       </c>
@@ -17278,7 +17281,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>727</v>
       </c>
@@ -17688,7 +17691,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>728</v>
       </c>
@@ -17765,7 +17768,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>730</v>
       </c>
@@ -18175,7 +18178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>731</v>
       </c>
@@ -18249,7 +18252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>732</v>
       </c>
@@ -18533,7 +18536,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>733</v>
       </c>
@@ -18817,7 +18820,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>734</v>
       </c>
@@ -19098,7 +19101,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>735</v>
       </c>
@@ -19511,7 +19514,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>736</v>
       </c>
@@ -19801,7 +19804,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>737</v>
       </c>
@@ -20076,7 +20079,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>739</v>
       </c>
@@ -20504,7 +20507,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>740</v>
       </c>
@@ -20779,7 +20782,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>741</v>
       </c>
@@ -20823,7 +20826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>742</v>
       </c>
@@ -20897,7 +20900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>743</v>
       </c>
@@ -20941,7 +20944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>744</v>
       </c>
@@ -21360,7 +21363,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>745</v>
       </c>
@@ -21404,7 +21407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>747</v>
       </c>
@@ -21484,7 +21487,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>748</v>
       </c>
@@ -21765,7 +21768,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>749</v>
       </c>
@@ -22043,7 +22046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>750</v>
       </c>
@@ -22462,7 +22465,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>751</v>
       </c>
@@ -22734,7 +22737,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>752</v>
       </c>
@@ -22778,7 +22781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>754</v>
       </c>
@@ -22849,7 +22852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>756</v>
       </c>
@@ -23133,7 +23136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>757</v>
       </c>
@@ -23546,7 +23549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>758</v>
       </c>
@@ -23617,7 +23620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>759</v>
       </c>
@@ -24024,7 +24027,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>760</v>
       </c>
@@ -24416,7 +24419,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>761</v>
       </c>
@@ -24826,7 +24829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>762</v>
       </c>
@@ -25245,7 +25248,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>763</v>
       </c>
@@ -25484,7 +25487,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>764</v>
       </c>
@@ -25765,7 +25768,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>767</v>
       </c>
@@ -26166,7 +26169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>768</v>
       </c>
@@ -26444,7 +26447,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>769</v>
       </c>
@@ -26719,7 +26722,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>770</v>
       </c>
@@ -26793,7 +26796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>771</v>
       </c>
@@ -26897,7 +26900,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>772</v>
       </c>
@@ -27169,7 +27172,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>773</v>
       </c>
@@ -27450,7 +27453,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>774</v>
       </c>
@@ -27734,7 +27737,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>775</v>
       </c>
@@ -27778,7 +27781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>779</v>
       </c>
@@ -27822,7 +27825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>780</v>
       </c>
@@ -28097,7 +28100,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>781</v>
       </c>
@@ -28204,7 +28207,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>782</v>
       </c>
@@ -28488,7 +28491,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>784</v>
       </c>
@@ -28895,7 +28898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>785</v>
       </c>
@@ -29314,7 +29317,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>786</v>
       </c>
@@ -29385,7 +29388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>787</v>
       </c>
@@ -29672,7 +29675,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>788</v>
       </c>
@@ -29956,7 +29959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>789</v>
       </c>
@@ -30234,7 +30237,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>791</v>
       </c>
@@ -30509,7 +30512,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>792</v>
       </c>
@@ -30940,7 +30943,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>793</v>
       </c>
@@ -31215,7 +31218,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>794</v>
       </c>
@@ -31490,7 +31493,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>795</v>
       </c>
@@ -31534,7 +31537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>797</v>
       </c>
@@ -31578,7 +31581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>799</v>
       </c>
@@ -31976,7 +31979,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>801</v>
       </c>
@@ -32251,7 +32254,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>802</v>
       </c>
@@ -32322,7 +32325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>803</v>
       </c>
@@ -32732,7 +32735,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>804</v>
       </c>
@@ -33007,7 +33010,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>805</v>
       </c>
@@ -33288,7 +33291,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>806</v>
       </c>
@@ -33572,7 +33575,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>807</v>
       </c>
@@ -33646,7 +33649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>808</v>
       </c>
@@ -33750,7 +33753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>809</v>
       </c>
@@ -33824,7 +33827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>811</v>
       </c>
@@ -33898,7 +33901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>812</v>
       </c>
@@ -33942,7 +33945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>813</v>
       </c>
@@ -34361,7 +34364,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>814</v>
       </c>
@@ -34465,7 +34468,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>815</v>
       </c>
@@ -34875,7 +34878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>816</v>
       </c>
@@ -35156,7 +35159,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>817</v>
       </c>
@@ -35434,7 +35437,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>819</v>
       </c>
@@ -35658,7 +35661,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>821</v>
       </c>
@@ -35942,7 +35945,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>823</v>
       </c>
@@ -35986,7 +35989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>824</v>
       </c>
@@ -36096,7 +36099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>825</v>
       </c>
@@ -36359,7 +36362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="124" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>828</v>
       </c>
@@ -36766,7 +36769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>829</v>
       </c>
@@ -37176,7 +37179,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>830</v>
       </c>
@@ -37589,7 +37592,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>831</v>
       </c>
@@ -37993,7 +37996,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>832</v>
       </c>
@@ -38403,7 +38406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>833</v>
       </c>
@@ -38681,7 +38684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>834</v>
       </c>
@@ -39091,7 +39094,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>836</v>
       </c>
@@ -39165,7 +39168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>837</v>
       </c>
@@ -39575,7 +39578,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>838</v>
       </c>
@@ -39619,7 +39622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>839</v>
       </c>
@@ -39663,7 +39666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>840</v>
       </c>
@@ -39737,7 +39740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>841</v>
       </c>
@@ -40147,7 +40150,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>842</v>
       </c>
@@ -40557,7 +40560,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>844</v>
       </c>
@@ -40601,7 +40604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>846</v>
       </c>
@@ -40816,7 +40819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>847</v>
       </c>
@@ -40860,7 +40863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>850</v>
       </c>
@@ -41129,7 +41132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>851</v>
       </c>
@@ -41407,7 +41410,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="143" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>852</v>
       </c>
@@ -41817,7 +41820,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>853</v>
       </c>
@@ -42227,7 +42230,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>854</v>
       </c>
@@ -42640,7 +42643,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>855</v>
       </c>
@@ -43050,7 +43053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="147" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>857</v>
       </c>
@@ -43463,7 +43466,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="148" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>858</v>
       </c>
@@ -43738,7 +43741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="149" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>859</v>
       </c>
@@ -44049,16 +44052,16 @@
         <v>1</v>
       </c>
       <c r="IG149" t="s">
+        <v>1834</v>
+      </c>
+      <c r="IH149" t="s">
         <v>1632</v>
       </c>
-      <c r="IH149" t="s">
+      <c r="II149" t="s">
         <v>1633</v>
       </c>
-      <c r="II149" t="s">
+      <c r="IJ149" t="s">
         <v>1634</v>
-      </c>
-      <c r="IJ149" t="s">
-        <v>1635</v>
       </c>
       <c r="MZ149">
         <v>4</v>
@@ -44148,7 +44151,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="150" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>860</v>
       </c>
@@ -44192,7 +44195,7 @@
         <v>1</v>
       </c>
       <c r="AS150" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="BF150">
         <v>6</v>
@@ -44219,34 +44222,34 @@
         <v>1</v>
       </c>
       <c r="CI150" t="s">
+        <v>1636</v>
+      </c>
+      <c r="DD150">
+        <v>2</v>
+      </c>
+      <c r="DE150">
+        <v>2</v>
+      </c>
+      <c r="DF150">
+        <v>1</v>
+      </c>
+      <c r="DG150">
+        <v>1</v>
+      </c>
+      <c r="DH150">
+        <v>1</v>
+      </c>
+      <c r="DI150">
+        <v>2</v>
+      </c>
+      <c r="DJ150">
+        <v>1</v>
+      </c>
+      <c r="DK150">
+        <v>1</v>
+      </c>
+      <c r="DY150" t="s">
         <v>1637</v>
-      </c>
-      <c r="DD150">
-        <v>2</v>
-      </c>
-      <c r="DE150">
-        <v>2</v>
-      </c>
-      <c r="DF150">
-        <v>1</v>
-      </c>
-      <c r="DG150">
-        <v>1</v>
-      </c>
-      <c r="DH150">
-        <v>1</v>
-      </c>
-      <c r="DI150">
-        <v>2</v>
-      </c>
-      <c r="DJ150">
-        <v>1</v>
-      </c>
-      <c r="DK150">
-        <v>1</v>
-      </c>
-      <c r="DY150" t="s">
-        <v>1638</v>
       </c>
       <c r="FB150" t="s">
         <v>628</v>
@@ -44273,7 +44276,7 @@
         <v>1</v>
       </c>
       <c r="FO150" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="FP150">
         <v>21</v>
@@ -44339,10 +44342,10 @@
         <v>800</v>
       </c>
       <c r="GO150" t="s">
+        <v>1639</v>
+      </c>
+      <c r="GP150" t="s">
         <v>1640</v>
-      </c>
-      <c r="GP150" t="s">
-        <v>1641</v>
       </c>
       <c r="GQ150" t="s">
         <v>840</v>
@@ -44354,7 +44357,7 @@
         <v>-9</v>
       </c>
       <c r="GV150" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="GW150">
         <v>0</v>
@@ -44456,16 +44459,16 @@
         <v>1</v>
       </c>
       <c r="IG150" t="s">
+        <v>1642</v>
+      </c>
+      <c r="IH150" t="s">
         <v>1643</v>
       </c>
-      <c r="IH150" t="s">
+      <c r="II150" t="s">
         <v>1644</v>
       </c>
-      <c r="II150" t="s">
+      <c r="IJ150" t="s">
         <v>1645</v>
-      </c>
-      <c r="IJ150" t="s">
-        <v>1646</v>
       </c>
       <c r="MZ150">
         <v>34</v>
@@ -44555,7 +44558,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>861</v>
       </c>
@@ -44659,7 +44662,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="152" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>862</v>
       </c>
@@ -44721,10 +44724,10 @@
         <v>2</v>
       </c>
       <c r="EI152" t="s">
+        <v>1646</v>
+      </c>
+      <c r="FL152" t="s">
         <v>1647</v>
-      </c>
-      <c r="FL152" t="s">
-        <v>1648</v>
       </c>
       <c r="FP152">
         <v>21</v>
@@ -44796,7 +44799,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="153" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>867</v>
       </c>
@@ -44837,34 +44840,34 @@
         <v>1</v>
       </c>
       <c r="AV153" t="s">
+        <v>1648</v>
+      </c>
+      <c r="BO153">
+        <v>2</v>
+      </c>
+      <c r="BP153">
+        <v>1</v>
+      </c>
+      <c r="BQ153">
+        <v>1</v>
+      </c>
+      <c r="BR153">
+        <v>2</v>
+      </c>
+      <c r="BS153">
+        <v>1</v>
+      </c>
+      <c r="BT153">
+        <v>1</v>
+      </c>
+      <c r="BU153">
+        <v>1</v>
+      </c>
+      <c r="BV153">
+        <v>1</v>
+      </c>
+      <c r="CJ153" t="s">
         <v>1649</v>
-      </c>
-      <c r="BO153">
-        <v>2</v>
-      </c>
-      <c r="BP153">
-        <v>1</v>
-      </c>
-      <c r="BQ153">
-        <v>1</v>
-      </c>
-      <c r="BR153">
-        <v>2</v>
-      </c>
-      <c r="BS153">
-        <v>1</v>
-      </c>
-      <c r="BT153">
-        <v>1</v>
-      </c>
-      <c r="BU153">
-        <v>1</v>
-      </c>
-      <c r="BV153">
-        <v>1</v>
-      </c>
-      <c r="CJ153" t="s">
-        <v>1650</v>
       </c>
       <c r="CU153">
         <v>120</v>
@@ -44891,7 +44894,7 @@
         <v>1</v>
       </c>
       <c r="DX153" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="EA153" t="s">
         <v>679</v>
@@ -44921,7 +44924,7 @@
         <v>2</v>
       </c>
       <c r="FL153" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="FP153">
         <v>21</v>
@@ -45002,10 +45005,10 @@
         <v>2</v>
       </c>
       <c r="GU153" t="s">
+        <v>1652</v>
+      </c>
+      <c r="GV153" t="s">
         <v>1653</v>
-      </c>
-      <c r="GV153" t="s">
-        <v>1654</v>
       </c>
       <c r="GW153">
         <v>1</v>
@@ -45074,7 +45077,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="154" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>868</v>
       </c>
@@ -45115,40 +45118,40 @@
         <v>1</v>
       </c>
       <c r="AU154" t="s">
+        <v>1654</v>
+      </c>
+      <c r="BX154" t="s">
         <v>1655</v>
       </c>
-      <c r="BX154" t="s">
+      <c r="BY154">
+        <v>2</v>
+      </c>
+      <c r="BZ154">
+        <v>1</v>
+      </c>
+      <c r="CA154">
+        <v>1</v>
+      </c>
+      <c r="CB154">
+        <v>1</v>
+      </c>
+      <c r="CC154">
+        <v>1</v>
+      </c>
+      <c r="CD154">
+        <v>1</v>
+      </c>
+      <c r="CE154">
+        <v>2</v>
+      </c>
+      <c r="CF154" t="s">
         <v>1656</v>
       </c>
-      <c r="BY154">
-        <v>2</v>
-      </c>
-      <c r="BZ154">
-        <v>1</v>
-      </c>
-      <c r="CA154">
-        <v>1</v>
-      </c>
-      <c r="CB154">
-        <v>1</v>
-      </c>
-      <c r="CC154">
-        <v>1</v>
-      </c>
-      <c r="CD154">
-        <v>1</v>
-      </c>
-      <c r="CE154">
-        <v>2</v>
-      </c>
-      <c r="CF154" t="s">
+      <c r="CK154" t="s">
         <v>1657</v>
       </c>
-      <c r="CK154" t="s">
+      <c r="CL154" t="s">
         <v>1658</v>
-      </c>
-      <c r="CL154" t="s">
-        <v>1659</v>
       </c>
       <c r="CM154">
         <v>4</v>
@@ -45172,13 +45175,13 @@
         <v>2</v>
       </c>
       <c r="CT154" t="s">
+        <v>1659</v>
+      </c>
+      <c r="DV154">
+        <v>2</v>
+      </c>
+      <c r="DW154" t="s">
         <v>1660</v>
-      </c>
-      <c r="DV154">
-        <v>2</v>
-      </c>
-      <c r="DW154" t="s">
-        <v>1661</v>
       </c>
       <c r="EJ154">
         <v>6</v>
@@ -45205,7 +45208,7 @@
         <v>1</v>
       </c>
       <c r="FM154" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="FP154">
         <v>22</v>
@@ -45271,10 +45274,10 @@
         <v>800</v>
       </c>
       <c r="GO154" t="s">
+        <v>1662</v>
+      </c>
+      <c r="GP154" t="s">
         <v>1663</v>
-      </c>
-      <c r="GP154" t="s">
-        <v>1664</v>
       </c>
       <c r="GQ154" t="s">
         <v>938</v>
@@ -45286,10 +45289,10 @@
         <v>2</v>
       </c>
       <c r="GU154" t="s">
+        <v>1664</v>
+      </c>
+      <c r="GV154" t="s">
         <v>1665</v>
-      </c>
-      <c r="GV154" t="s">
-        <v>1666</v>
       </c>
       <c r="GW154">
         <v>1</v>
@@ -45358,7 +45361,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>870</v>
       </c>
@@ -45432,7 +45435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>871</v>
       </c>
@@ -45449,7 +45452,7 @@
         <v>44182.933240740742</v>
       </c>
       <c r="AW156" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="AX156">
         <v>3</v>
@@ -45473,10 +45476,10 @@
         <v>2</v>
       </c>
       <c r="BE156" t="s">
+        <v>1667</v>
+      </c>
+      <c r="ES156" t="s">
         <v>1668</v>
-      </c>
-      <c r="ES156" t="s">
-        <v>1669</v>
       </c>
       <c r="FP156">
         <v>22</v>
@@ -45545,7 +45548,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="157" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>872</v>
       </c>
@@ -45562,7 +45565,7 @@
         <v>44182.935254629629</v>
       </c>
       <c r="AI157" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="AJ157">
         <v>3</v>
@@ -45586,7 +45589,7 @@
         <v>1</v>
       </c>
       <c r="BO157" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="BP157">
         <v>3</v>
@@ -45610,7 +45613,7 @@
         <v>1</v>
       </c>
       <c r="CU157" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="CV157">
         <v>3</v>
@@ -45634,7 +45637,7 @@
         <v>1</v>
       </c>
       <c r="EA157" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="EB157">
         <v>3</v>
@@ -45706,7 +45709,7 @@
         <v>15</v>
       </c>
       <c r="GH157" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="GI157">
         <v>5</v>
@@ -45727,13 +45730,13 @@
         <v>800</v>
       </c>
       <c r="GO157" t="s">
+        <v>1674</v>
+      </c>
+      <c r="GP157" t="s">
         <v>1675</v>
       </c>
-      <c r="GP157" t="s">
+      <c r="GQ157" t="s">
         <v>1676</v>
-      </c>
-      <c r="GQ157" t="s">
-        <v>1677</v>
       </c>
       <c r="GR157" t="s">
         <v>604</v>
@@ -45742,10 +45745,10 @@
         <v>2</v>
       </c>
       <c r="GU157" t="s">
+        <v>1677</v>
+      </c>
+      <c r="GV157" t="s">
         <v>1678</v>
-      </c>
-      <c r="GV157" t="s">
-        <v>1679</v>
       </c>
       <c r="GW157">
         <v>0</v>
@@ -45814,7 +45817,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>873</v>
       </c>
@@ -45915,7 +45918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>874</v>
       </c>
@@ -45989,7 +45992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>875</v>
       </c>
@@ -46030,37 +46033,37 @@
         <v>1</v>
       </c>
       <c r="AT160" t="s">
+        <v>1679</v>
+      </c>
+      <c r="AW160" t="s">
         <v>1680</v>
       </c>
-      <c r="AW160" t="s">
+      <c r="AX160">
+        <v>1</v>
+      </c>
+      <c r="AY160">
+        <v>1</v>
+      </c>
+      <c r="AZ160">
+        <v>2</v>
+      </c>
+      <c r="BA160">
+        <v>1</v>
+      </c>
+      <c r="BB160">
+        <v>1</v>
+      </c>
+      <c r="BC160">
+        <v>1</v>
+      </c>
+      <c r="BD160">
+        <v>1</v>
+      </c>
+      <c r="CG160">
+        <v>1</v>
+      </c>
+      <c r="CH160" t="s">
         <v>1681</v>
-      </c>
-      <c r="AX160">
-        <v>1</v>
-      </c>
-      <c r="AY160">
-        <v>1</v>
-      </c>
-      <c r="AZ160">
-        <v>2</v>
-      </c>
-      <c r="BA160">
-        <v>1</v>
-      </c>
-      <c r="BB160">
-        <v>1</v>
-      </c>
-      <c r="BC160">
-        <v>1</v>
-      </c>
-      <c r="BD160">
-        <v>1</v>
-      </c>
-      <c r="CG160">
-        <v>1</v>
-      </c>
-      <c r="CH160" t="s">
-        <v>1682</v>
       </c>
       <c r="DM160" t="s">
         <v>628</v>
@@ -46087,34 +46090,34 @@
         <v>1</v>
       </c>
       <c r="DZ160" t="s">
+        <v>1682</v>
+      </c>
+      <c r="ES160">
+        <v>2</v>
+      </c>
+      <c r="ET160">
+        <v>1</v>
+      </c>
+      <c r="EU160">
+        <v>1</v>
+      </c>
+      <c r="EV160">
+        <v>2</v>
+      </c>
+      <c r="EW160">
+        <v>1</v>
+      </c>
+      <c r="EX160">
+        <v>1</v>
+      </c>
+      <c r="EY160">
+        <v>1</v>
+      </c>
+      <c r="EZ160">
+        <v>1</v>
+      </c>
+      <c r="FN160" t="s">
         <v>1683</v>
-      </c>
-      <c r="ES160">
-        <v>2</v>
-      </c>
-      <c r="ET160">
-        <v>1</v>
-      </c>
-      <c r="EU160">
-        <v>1</v>
-      </c>
-      <c r="EV160">
-        <v>2</v>
-      </c>
-      <c r="EW160">
-        <v>1</v>
-      </c>
-      <c r="EX160">
-        <v>1</v>
-      </c>
-      <c r="EY160">
-        <v>1</v>
-      </c>
-      <c r="EZ160">
-        <v>1</v>
-      </c>
-      <c r="FN160" t="s">
-        <v>1684</v>
       </c>
       <c r="FP160">
         <v>22</v>
@@ -46162,7 +46165,7 @@
         <v>-2</v>
       </c>
       <c r="GH160" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="GI160">
         <v>-2</v>
@@ -46180,13 +46183,13 @@
         <v>800</v>
       </c>
       <c r="GO160" t="s">
+        <v>1685</v>
+      </c>
+      <c r="GP160" t="s">
         <v>1686</v>
       </c>
-      <c r="GP160" t="s">
+      <c r="GQ160" t="s">
         <v>1687</v>
-      </c>
-      <c r="GQ160" t="s">
-        <v>1688</v>
       </c>
       <c r="GR160" t="s">
         <v>604</v>
@@ -46195,7 +46198,7 @@
         <v>-9</v>
       </c>
       <c r="GV160" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="GW160">
         <v>1</v>
@@ -46297,16 +46300,16 @@
         <v>1</v>
       </c>
       <c r="JU160" t="s">
+        <v>1689</v>
+      </c>
+      <c r="JV160" t="s">
         <v>1690</v>
       </c>
-      <c r="JV160" t="s">
+      <c r="JW160" t="s">
         <v>1691</v>
       </c>
-      <c r="JW160" t="s">
+      <c r="JX160" t="s">
         <v>1692</v>
-      </c>
-      <c r="JX160" t="s">
-        <v>1693</v>
       </c>
       <c r="MZ160">
         <v>19</v>
@@ -46396,7 +46399,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="161" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>876</v>
       </c>
@@ -46437,7 +46440,7 @@
         <v>1</v>
       </c>
       <c r="AT161" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="AW161">
         <v>31623426175536</v>
@@ -46467,7 +46470,7 @@
         <v>1</v>
       </c>
       <c r="CH161" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="DM161" t="s">
         <v>628</v>
@@ -46494,7 +46497,7 @@
         <v>1</v>
       </c>
       <c r="DZ161" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="ES161">
         <v>2</v>
@@ -46521,7 +46524,7 @@
         <v>1</v>
       </c>
       <c r="FN161" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="FP161">
         <v>22</v>
@@ -46587,13 +46590,13 @@
         <v>800</v>
       </c>
       <c r="GO161" t="s">
+        <v>1697</v>
+      </c>
+      <c r="GP161" t="s">
         <v>1698</v>
       </c>
-      <c r="GP161" t="s">
-        <v>1699</v>
-      </c>
       <c r="GQ161" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="GR161" t="s">
         <v>604</v>
@@ -46602,7 +46605,7 @@
         <v>-9</v>
       </c>
       <c r="GV161" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="GW161">
         <v>1</v>
@@ -46656,7 +46659,7 @@
         <v>1</v>
       </c>
       <c r="JC161" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="JD161">
         <v>5</v>
@@ -46704,16 +46707,16 @@
         <v>1</v>
       </c>
       <c r="JU161" t="s">
+        <v>1701</v>
+      </c>
+      <c r="JV161" t="s">
         <v>1702</v>
       </c>
-      <c r="JV161" t="s">
+      <c r="JW161" t="s">
         <v>1703</v>
       </c>
-      <c r="JW161" t="s">
+      <c r="JX161" t="s">
         <v>1704</v>
-      </c>
-      <c r="JX161" t="s">
-        <v>1705</v>
       </c>
       <c r="MZ161">
         <v>3</v>
@@ -46803,7 +46806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="162" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>877</v>
       </c>
@@ -46841,34 +46844,34 @@
         <v>1</v>
       </c>
       <c r="AU162" t="s">
+        <v>1705</v>
+      </c>
+      <c r="BX162" t="s">
         <v>1706</v>
       </c>
-      <c r="BX162" t="s">
+      <c r="BY162">
+        <v>2</v>
+      </c>
+      <c r="BZ162">
+        <v>1</v>
+      </c>
+      <c r="CA162">
+        <v>1</v>
+      </c>
+      <c r="CB162">
+        <v>1</v>
+      </c>
+      <c r="CC162">
+        <v>2</v>
+      </c>
+      <c r="CD162">
+        <v>1</v>
+      </c>
+      <c r="CE162">
+        <v>1</v>
+      </c>
+      <c r="CK162" t="s">
         <v>1707</v>
-      </c>
-      <c r="BY162">
-        <v>2</v>
-      </c>
-      <c r="BZ162">
-        <v>1</v>
-      </c>
-      <c r="CA162">
-        <v>1</v>
-      </c>
-      <c r="CB162">
-        <v>1</v>
-      </c>
-      <c r="CC162">
-        <v>2</v>
-      </c>
-      <c r="CD162">
-        <v>1</v>
-      </c>
-      <c r="CE162">
-        <v>1</v>
-      </c>
-      <c r="CK162" t="s">
-        <v>1708</v>
       </c>
       <c r="CL162">
         <v>31623427561536</v>
@@ -46898,7 +46901,7 @@
         <v>2</v>
       </c>
       <c r="DW162" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="EJ162">
         <v>6</v>
@@ -46925,7 +46928,7 @@
         <v>1</v>
       </c>
       <c r="FM162" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="FP162">
         <v>23</v>
@@ -46991,13 +46994,13 @@
         <v>800</v>
       </c>
       <c r="GO162" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="GP162" t="s">
         <v>644</v>
       </c>
       <c r="GQ162" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="GR162" t="s">
         <v>604</v>
@@ -47006,7 +47009,7 @@
         <v>-9</v>
       </c>
       <c r="GV162" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="GW162">
         <v>0</v>
@@ -47075,7 +47078,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>878</v>
       </c>
@@ -47113,7 +47116,7 @@
         <v>1</v>
       </c>
       <c r="AV163" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="BO163">
         <v>23</v>
@@ -47140,7 +47143,7 @@
         <v>1</v>
       </c>
       <c r="CJ163" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="EA163">
         <v>536</v>
@@ -47167,7 +47170,7 @@
         <v>1</v>
       </c>
       <c r="FL163" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="FP163">
         <v>23</v>
@@ -47245,7 +47248,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="164" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>879</v>
       </c>
@@ -47289,7 +47292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>880</v>
       </c>
@@ -47330,7 +47333,7 @@
         <v>1</v>
       </c>
       <c r="AV165" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="BO165">
         <v>3</v>
@@ -47357,7 +47360,7 @@
         <v>1</v>
       </c>
       <c r="CJ165" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="CU165">
         <v>120</v>
@@ -47384,7 +47387,7 @@
         <v>1</v>
       </c>
       <c r="DX165" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="EA165">
         <v>31623426175536</v>
@@ -47414,7 +47417,7 @@
         <v>1</v>
       </c>
       <c r="FL165" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="FP165">
         <v>23</v>
@@ -47462,7 +47465,7 @@
         <v>-2</v>
       </c>
       <c r="GH165" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="GI165">
         <v>-2</v>
@@ -47480,10 +47483,10 @@
         <v>800</v>
       </c>
       <c r="GO165" t="s">
+        <v>1721</v>
+      </c>
+      <c r="GP165" t="s">
         <v>1722</v>
-      </c>
-      <c r="GP165" t="s">
-        <v>1723</v>
       </c>
       <c r="GQ165" t="s">
         <v>665</v>
@@ -47495,7 +47498,7 @@
         <v>-9</v>
       </c>
       <c r="GV165" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="GW165">
         <v>0</v>
@@ -47591,16 +47594,16 @@
         <v>1</v>
       </c>
       <c r="MV165" t="s">
+        <v>1724</v>
+      </c>
+      <c r="MW165" t="s">
         <v>1725</v>
       </c>
-      <c r="MW165" t="s">
+      <c r="MX165" t="s">
         <v>1726</v>
       </c>
-      <c r="MX165" t="s">
+      <c r="MY165" t="s">
         <v>1727</v>
-      </c>
-      <c r="MY165" t="s">
-        <v>1728</v>
       </c>
       <c r="MZ165">
         <v>3</v>
@@ -47690,7 +47693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="166" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>881</v>
       </c>
@@ -47764,7 +47767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>882</v>
       </c>
@@ -48057,7 +48060,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>883</v>
       </c>
@@ -48101,7 +48104,7 @@
         <v>2</v>
       </c>
       <c r="AS168" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="BF168">
         <v>6</v>
@@ -48128,34 +48131,34 @@
         <v>1</v>
       </c>
       <c r="CI168" t="s">
+        <v>1729</v>
+      </c>
+      <c r="DD168">
+        <v>1</v>
+      </c>
+      <c r="DE168">
+        <v>2</v>
+      </c>
+      <c r="DF168">
+        <v>1</v>
+      </c>
+      <c r="DG168">
+        <v>1</v>
+      </c>
+      <c r="DH168">
+        <v>2</v>
+      </c>
+      <c r="DI168">
+        <v>1</v>
+      </c>
+      <c r="DJ168">
+        <v>1</v>
+      </c>
+      <c r="DK168">
+        <v>1</v>
+      </c>
+      <c r="DY168" t="s">
         <v>1730</v>
-      </c>
-      <c r="DD168">
-        <v>1</v>
-      </c>
-      <c r="DE168">
-        <v>2</v>
-      </c>
-      <c r="DF168">
-        <v>1</v>
-      </c>
-      <c r="DG168">
-        <v>1</v>
-      </c>
-      <c r="DH168">
-        <v>2</v>
-      </c>
-      <c r="DI168">
-        <v>1</v>
-      </c>
-      <c r="DJ168">
-        <v>1</v>
-      </c>
-      <c r="DK168">
-        <v>1</v>
-      </c>
-      <c r="DY168" t="s">
-        <v>1731</v>
       </c>
       <c r="FB168">
         <v>11</v>
@@ -48182,7 +48185,7 @@
         <v>1</v>
       </c>
       <c r="FO168" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="FP168">
         <v>23</v>
@@ -48230,7 +48233,7 @@
         <v>-2</v>
       </c>
       <c r="GH168" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="GI168">
         <v>-2</v>
@@ -48248,10 +48251,10 @@
         <v>800</v>
       </c>
       <c r="GO168" t="s">
+        <v>1733</v>
+      </c>
+      <c r="GP168" t="s">
         <v>1734</v>
-      </c>
-      <c r="GP168" t="s">
-        <v>1735</v>
       </c>
       <c r="GQ168" t="s">
         <v>938</v>
@@ -48329,7 +48332,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>884</v>
       </c>
@@ -48373,7 +48376,7 @@
         <v>1</v>
       </c>
       <c r="AS169" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="BF169">
         <v>6</v>
@@ -48400,34 +48403,34 @@
         <v>1</v>
       </c>
       <c r="CI169" t="s">
+        <v>1736</v>
+      </c>
+      <c r="DD169">
+        <v>2</v>
+      </c>
+      <c r="DE169">
+        <v>1</v>
+      </c>
+      <c r="DF169">
+        <v>1</v>
+      </c>
+      <c r="DG169">
+        <v>1</v>
+      </c>
+      <c r="DH169">
+        <v>1</v>
+      </c>
+      <c r="DI169">
+        <v>2</v>
+      </c>
+      <c r="DJ169">
+        <v>1</v>
+      </c>
+      <c r="DK169">
+        <v>1</v>
+      </c>
+      <c r="DY169" t="s">
         <v>1737</v>
-      </c>
-      <c r="DD169">
-        <v>2</v>
-      </c>
-      <c r="DE169">
-        <v>1</v>
-      </c>
-      <c r="DF169">
-        <v>1</v>
-      </c>
-      <c r="DG169">
-        <v>1</v>
-      </c>
-      <c r="DH169">
-        <v>1</v>
-      </c>
-      <c r="DI169">
-        <v>2</v>
-      </c>
-      <c r="DJ169">
-        <v>1</v>
-      </c>
-      <c r="DK169">
-        <v>1</v>
-      </c>
-      <c r="DY169" t="s">
-        <v>1738</v>
       </c>
       <c r="FB169" t="s">
         <v>628</v>
@@ -48454,10 +48457,10 @@
         <v>2</v>
       </c>
       <c r="FJ169" t="s">
+        <v>1738</v>
+      </c>
+      <c r="FO169" t="s">
         <v>1739</v>
-      </c>
-      <c r="FO169" t="s">
-        <v>1740</v>
       </c>
       <c r="FP169">
         <v>23</v>
@@ -48514,7 +48517,7 @@
         <v>1</v>
       </c>
       <c r="II169" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="MZ169">
         <v>115</v>
@@ -48580,7 +48583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>885</v>
       </c>
@@ -48597,31 +48600,31 @@
         <v>44185.565428240741</v>
       </c>
       <c r="H170" t="s">
+        <v>1741</v>
+      </c>
+      <c r="I170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="K170">
+        <v>2</v>
+      </c>
+      <c r="L170">
+        <v>1</v>
+      </c>
+      <c r="M170">
+        <v>1</v>
+      </c>
+      <c r="N170">
+        <v>1</v>
+      </c>
+      <c r="O170">
+        <v>1</v>
+      </c>
+      <c r="AS170" t="s">
         <v>1742</v>
-      </c>
-      <c r="I170">
-        <v>1</v>
-      </c>
-      <c r="J170">
-        <v>1</v>
-      </c>
-      <c r="K170">
-        <v>2</v>
-      </c>
-      <c r="L170">
-        <v>1</v>
-      </c>
-      <c r="M170">
-        <v>1</v>
-      </c>
-      <c r="N170">
-        <v>1</v>
-      </c>
-      <c r="O170">
-        <v>1</v>
-      </c>
-      <c r="AS170" t="s">
-        <v>1743</v>
       </c>
       <c r="BF170">
         <v>6</v>
@@ -48648,7 +48651,7 @@
         <v>1</v>
       </c>
       <c r="CI170" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="FP170">
         <v>23</v>
@@ -48720,7 +48723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>886</v>
       </c>
@@ -48764,7 +48767,7 @@
         <v>1</v>
       </c>
       <c r="AS171" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="BF171">
         <v>6</v>
@@ -48791,34 +48794,34 @@
         <v>1</v>
       </c>
       <c r="CI171" t="s">
+        <v>1745</v>
+      </c>
+      <c r="DD171">
+        <v>2</v>
+      </c>
+      <c r="DE171">
+        <v>2</v>
+      </c>
+      <c r="DF171">
+        <v>1</v>
+      </c>
+      <c r="DG171">
+        <v>1</v>
+      </c>
+      <c r="DH171">
+        <v>2</v>
+      </c>
+      <c r="DI171">
+        <v>1</v>
+      </c>
+      <c r="DJ171">
+        <v>1</v>
+      </c>
+      <c r="DK171">
+        <v>1</v>
+      </c>
+      <c r="DY171" t="s">
         <v>1746</v>
-      </c>
-      <c r="DD171">
-        <v>2</v>
-      </c>
-      <c r="DE171">
-        <v>2</v>
-      </c>
-      <c r="DF171">
-        <v>1</v>
-      </c>
-      <c r="DG171">
-        <v>1</v>
-      </c>
-      <c r="DH171">
-        <v>2</v>
-      </c>
-      <c r="DI171">
-        <v>1</v>
-      </c>
-      <c r="DJ171">
-        <v>1</v>
-      </c>
-      <c r="DK171">
-        <v>1</v>
-      </c>
-      <c r="DY171" t="s">
-        <v>1747</v>
       </c>
       <c r="FB171" t="s">
         <v>628</v>
@@ -48845,7 +48848,7 @@
         <v>1</v>
       </c>
       <c r="FO171" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="FP171">
         <v>24</v>
@@ -48893,7 +48896,7 @@
         <v>-2</v>
       </c>
       <c r="GH171" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="GI171">
         <v>-2</v>
@@ -48914,7 +48917,7 @@
         <v>77180254195</v>
       </c>
       <c r="GP171" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="GQ171" t="s">
         <v>938</v>
@@ -48926,7 +48929,7 @@
         <v>2</v>
       </c>
       <c r="GU171" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="GW171">
         <v>1</v>
@@ -48956,7 +48959,7 @@
         <v>1</v>
       </c>
       <c r="HG171" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="HH171">
         <v>2</v>
@@ -49004,10 +49007,10 @@
         <v>2</v>
       </c>
       <c r="HW171" t="s">
+        <v>1752</v>
+      </c>
+      <c r="HX171" t="s">
         <v>1753</v>
-      </c>
-      <c r="HX171" t="s">
-        <v>1754</v>
       </c>
       <c r="HY171">
         <v>4</v>
@@ -49031,16 +49034,16 @@
         <v>1</v>
       </c>
       <c r="IG171" t="s">
+        <v>1754</v>
+      </c>
+      <c r="IH171" t="s">
         <v>1755</v>
       </c>
-      <c r="IH171" t="s">
+      <c r="II171" t="s">
         <v>1756</v>
       </c>
-      <c r="II171" t="s">
+      <c r="IJ171" t="s">
         <v>1757</v>
-      </c>
-      <c r="IJ171" t="s">
-        <v>1758</v>
       </c>
       <c r="MZ171">
         <v>1</v>
@@ -49130,7 +49133,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>888</v>
       </c>
@@ -49147,37 +49150,37 @@
         <v>44185.596226851849</v>
       </c>
       <c r="AI172" t="s">
+        <v>1758</v>
+      </c>
+      <c r="AJ172">
+        <v>2</v>
+      </c>
+      <c r="AK172">
+        <v>2</v>
+      </c>
+      <c r="AL172">
+        <v>1</v>
+      </c>
+      <c r="AM172">
+        <v>1</v>
+      </c>
+      <c r="AN172">
+        <v>1</v>
+      </c>
+      <c r="AO172">
+        <v>2</v>
+      </c>
+      <c r="AP172">
+        <v>2</v>
+      </c>
+      <c r="AQ172" t="s">
         <v>1759</v>
       </c>
-      <c r="AJ172">
-        <v>2</v>
-      </c>
-      <c r="AK172">
-        <v>2</v>
-      </c>
-      <c r="AL172">
-        <v>1</v>
-      </c>
-      <c r="AM172">
-        <v>1</v>
-      </c>
-      <c r="AN172">
-        <v>1</v>
-      </c>
-      <c r="AO172">
-        <v>2</v>
-      </c>
-      <c r="AP172">
-        <v>2</v>
-      </c>
-      <c r="AQ172" t="s">
+      <c r="AV172" t="s">
         <v>1760</v>
       </c>
-      <c r="AV172" t="s">
+      <c r="BO172" t="s">
         <v>1761</v>
-      </c>
-      <c r="BO172" t="s">
-        <v>1762</v>
       </c>
       <c r="BP172">
         <v>3</v>
@@ -49201,10 +49204,10 @@
         <v>2</v>
       </c>
       <c r="BW172" t="s">
+        <v>1762</v>
+      </c>
+      <c r="CJ172" t="s">
         <v>1763</v>
-      </c>
-      <c r="CJ172" t="s">
-        <v>1764</v>
       </c>
       <c r="CU172">
         <v>120</v>
@@ -49231,7 +49234,7 @@
         <v>1</v>
       </c>
       <c r="DX172" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="EA172" t="s">
         <v>641</v>
@@ -49261,7 +49264,7 @@
         <v>1</v>
       </c>
       <c r="FL172" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="FP172">
         <v>24</v>
@@ -49309,7 +49312,7 @@
         <v>20</v>
       </c>
       <c r="GH172" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="GI172">
         <v>5</v>
@@ -49330,10 +49333,10 @@
         <v>800</v>
       </c>
       <c r="GO172" t="s">
+        <v>1767</v>
+      </c>
+      <c r="GP172" t="s">
         <v>1768</v>
-      </c>
-      <c r="GP172" t="s">
-        <v>1769</v>
       </c>
       <c r="GQ172" t="s">
         <v>603</v>
@@ -49345,91 +49348,91 @@
         <v>2</v>
       </c>
       <c r="GU172" t="s">
+        <v>1769</v>
+      </c>
+      <c r="GV172" t="s">
         <v>1770</v>
       </c>
-      <c r="GV172" t="s">
+      <c r="GW172">
+        <v>1</v>
+      </c>
+      <c r="LM172" t="s">
         <v>1771</v>
       </c>
-      <c r="GW172">
-        <v>1</v>
-      </c>
-      <c r="LM172" t="s">
+      <c r="LN172">
+        <v>1</v>
+      </c>
+      <c r="LO172">
+        <v>1</v>
+      </c>
+      <c r="LP172">
+        <v>1</v>
+      </c>
+      <c r="LQ172">
+        <v>1</v>
+      </c>
+      <c r="LR172">
+        <v>1</v>
+      </c>
+      <c r="LS172">
+        <v>1</v>
+      </c>
+      <c r="LT172">
+        <v>2</v>
+      </c>
+      <c r="LU172" t="s">
         <v>1772</v>
       </c>
-      <c r="LN172">
-        <v>1</v>
-      </c>
-      <c r="LO172">
-        <v>1</v>
-      </c>
-      <c r="LP172">
-        <v>1</v>
-      </c>
-      <c r="LQ172">
-        <v>1</v>
-      </c>
-      <c r="LR172">
-        <v>1</v>
-      </c>
-      <c r="LS172">
-        <v>1</v>
-      </c>
-      <c r="LT172">
-        <v>2</v>
-      </c>
-      <c r="LU172" t="s">
+      <c r="LV172" t="s">
         <v>1773</v>
       </c>
-      <c r="LV172" t="s">
+      <c r="LW172">
+        <v>1</v>
+      </c>
+      <c r="LX172">
+        <v>1</v>
+      </c>
+      <c r="LY172">
+        <v>2</v>
+      </c>
+      <c r="LZ172">
+        <v>1</v>
+      </c>
+      <c r="MA172">
+        <v>1</v>
+      </c>
+      <c r="MB172">
+        <v>1</v>
+      </c>
+      <c r="MC172">
+        <v>1</v>
+      </c>
+      <c r="ME172" t="s">
         <v>1774</v>
       </c>
-      <c r="LW172">
-        <v>1</v>
-      </c>
-      <c r="LX172">
-        <v>1</v>
-      </c>
-      <c r="LY172">
-        <v>2</v>
-      </c>
-      <c r="LZ172">
-        <v>1</v>
-      </c>
-      <c r="MA172">
-        <v>1</v>
-      </c>
-      <c r="MB172">
-        <v>1</v>
-      </c>
-      <c r="MC172">
-        <v>1</v>
-      </c>
-      <c r="ME172" t="s">
+      <c r="MF172">
+        <v>1</v>
+      </c>
+      <c r="MG172">
+        <v>1</v>
+      </c>
+      <c r="MH172">
+        <v>2</v>
+      </c>
+      <c r="MI172">
+        <v>1</v>
+      </c>
+      <c r="MJ172">
+        <v>1</v>
+      </c>
+      <c r="MK172">
+        <v>1</v>
+      </c>
+      <c r="ML172">
+        <v>1</v>
+      </c>
+      <c r="MN172" t="s">
         <v>1775</v>
-      </c>
-      <c r="MF172">
-        <v>1</v>
-      </c>
-      <c r="MG172">
-        <v>1</v>
-      </c>
-      <c r="MH172">
-        <v>2</v>
-      </c>
-      <c r="MI172">
-        <v>1</v>
-      </c>
-      <c r="MJ172">
-        <v>1</v>
-      </c>
-      <c r="MK172">
-        <v>1</v>
-      </c>
-      <c r="ML172">
-        <v>1</v>
-      </c>
-      <c r="MN172" t="s">
-        <v>1776</v>
       </c>
       <c r="MO172">
         <v>4</v>
@@ -49453,16 +49456,16 @@
         <v>1</v>
       </c>
       <c r="MV172" t="s">
+        <v>1776</v>
+      </c>
+      <c r="MW172" t="s">
         <v>1777</v>
       </c>
-      <c r="MW172" t="s">
+      <c r="MX172" t="s">
         <v>1778</v>
       </c>
-      <c r="MX172" t="s">
+      <c r="MY172" t="s">
         <v>1779</v>
-      </c>
-      <c r="MY172" t="s">
-        <v>1780</v>
       </c>
       <c r="MZ172">
         <v>29</v>
@@ -49552,7 +49555,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>889</v>
       </c>
@@ -49593,7 +49596,7 @@
         <v>1</v>
       </c>
       <c r="AU173" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="BX173" t="s">
         <v>636</v>
@@ -49620,7 +49623,7 @@
         <v>1</v>
       </c>
       <c r="CK173" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="CL173" t="s">
         <v>641</v>
@@ -49650,7 +49653,7 @@
         <v>2</v>
       </c>
       <c r="DW173" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="EJ173">
         <v>6</v>
@@ -49677,7 +49680,7 @@
         <v>1</v>
       </c>
       <c r="FM173" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="FP173">
         <v>24</v>
@@ -49725,7 +49728,7 @@
         <v>-2</v>
       </c>
       <c r="GH173" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="GI173">
         <v>-2</v>
@@ -49743,10 +49746,10 @@
         <v>800</v>
       </c>
       <c r="GO173" t="s">
+        <v>1785</v>
+      </c>
+      <c r="GP173" t="s">
         <v>1786</v>
-      </c>
-      <c r="GP173" t="s">
-        <v>1787</v>
       </c>
       <c r="GQ173" t="s">
         <v>665</v>
@@ -49758,7 +49761,7 @@
         <v>1</v>
       </c>
       <c r="GV173" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="GW173">
         <v>0</v>
@@ -49827,7 +49830,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="174" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>890</v>
       </c>
@@ -49919,7 +49922,7 @@
         <v>1</v>
       </c>
       <c r="DZ174" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="ES174">
         <v>2</v>
@@ -50009,10 +50012,10 @@
         <v>355</v>
       </c>
       <c r="GO174" t="s">
+        <v>1789</v>
+      </c>
+      <c r="GP174" t="s">
         <v>1790</v>
-      </c>
-      <c r="GP174" t="s">
-        <v>1791</v>
       </c>
       <c r="GQ174" t="s">
         <v>938</v>
@@ -50024,7 +50027,7 @@
         <v>-9</v>
       </c>
       <c r="GV174" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="GW174">
         <v>1</v>
@@ -50093,7 +50096,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>891</v>
       </c>
@@ -50167,7 +50170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>892</v>
       </c>
@@ -50241,7 +50244,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>893</v>
       </c>
@@ -50282,7 +50285,7 @@
         <v>1</v>
       </c>
       <c r="AT177" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="AW177">
         <v>61</v>
@@ -50312,7 +50315,7 @@
         <v>1</v>
       </c>
       <c r="CH177" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="DM177" t="s">
         <v>628</v>
@@ -50339,34 +50342,34 @@
         <v>1</v>
       </c>
       <c r="DZ177" t="s">
+        <v>1794</v>
+      </c>
+      <c r="ES177">
+        <v>2</v>
+      </c>
+      <c r="ET177">
+        <v>1</v>
+      </c>
+      <c r="EU177">
+        <v>1</v>
+      </c>
+      <c r="EV177">
+        <v>2</v>
+      </c>
+      <c r="EW177">
+        <v>1</v>
+      </c>
+      <c r="EX177">
+        <v>1</v>
+      </c>
+      <c r="EY177">
+        <v>1</v>
+      </c>
+      <c r="EZ177">
+        <v>1</v>
+      </c>
+      <c r="FN177" t="s">
         <v>1795</v>
-      </c>
-      <c r="ES177">
-        <v>2</v>
-      </c>
-      <c r="ET177">
-        <v>1</v>
-      </c>
-      <c r="EU177">
-        <v>1</v>
-      </c>
-      <c r="EV177">
-        <v>2</v>
-      </c>
-      <c r="EW177">
-        <v>1</v>
-      </c>
-      <c r="EX177">
-        <v>1</v>
-      </c>
-      <c r="EY177">
-        <v>1</v>
-      </c>
-      <c r="EZ177">
-        <v>1</v>
-      </c>
-      <c r="FN177" t="s">
-        <v>1796</v>
       </c>
       <c r="FP177">
         <v>25</v>
@@ -50453,7 +50456,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="178" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>894</v>
       </c>
@@ -50497,7 +50500,7 @@
         <v>2</v>
       </c>
       <c r="AS178" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="BF178">
         <v>6</v>
@@ -50524,34 +50527,34 @@
         <v>1</v>
       </c>
       <c r="CI178" t="s">
+        <v>1797</v>
+      </c>
+      <c r="DD178">
+        <v>2</v>
+      </c>
+      <c r="DE178">
+        <v>1</v>
+      </c>
+      <c r="DF178">
+        <v>1</v>
+      </c>
+      <c r="DG178">
+        <v>2</v>
+      </c>
+      <c r="DH178">
+        <v>1</v>
+      </c>
+      <c r="DI178">
+        <v>1</v>
+      </c>
+      <c r="DJ178">
+        <v>1</v>
+      </c>
+      <c r="DK178">
+        <v>1</v>
+      </c>
+      <c r="DY178" t="s">
         <v>1798</v>
-      </c>
-      <c r="DD178">
-        <v>2</v>
-      </c>
-      <c r="DE178">
-        <v>1</v>
-      </c>
-      <c r="DF178">
-        <v>1</v>
-      </c>
-      <c r="DG178">
-        <v>2</v>
-      </c>
-      <c r="DH178">
-        <v>1</v>
-      </c>
-      <c r="DI178">
-        <v>1</v>
-      </c>
-      <c r="DJ178">
-        <v>1</v>
-      </c>
-      <c r="DK178">
-        <v>1</v>
-      </c>
-      <c r="DY178" t="s">
-        <v>1799</v>
       </c>
       <c r="FB178" t="s">
         <v>628</v>
@@ -50578,7 +50581,7 @@
         <v>1</v>
       </c>
       <c r="FO178" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="FP178">
         <v>25</v>
@@ -50626,7 +50629,7 @@
         <v>15</v>
       </c>
       <c r="GH178" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="GI178">
         <v>5</v>
@@ -50662,7 +50665,7 @@
         <v>-9</v>
       </c>
       <c r="GV178" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="GW178">
         <v>1</v>
@@ -50731,7 +50734,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="179" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>895</v>
       </c>
@@ -50772,7 +50775,7 @@
         <v>1</v>
       </c>
       <c r="AU179" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="BX179" t="s">
         <v>636</v>
@@ -50799,10 +50802,10 @@
         <v>2</v>
       </c>
       <c r="CF179" t="s">
+        <v>1802</v>
+      </c>
+      <c r="CK179" t="s">
         <v>1803</v>
-      </c>
-      <c r="CK179" t="s">
-        <v>1804</v>
       </c>
       <c r="CL179" t="s">
         <v>641</v>
@@ -50829,13 +50832,13 @@
         <v>2</v>
       </c>
       <c r="CT179" t="s">
+        <v>1804</v>
+      </c>
+      <c r="DV179">
+        <v>2</v>
+      </c>
+      <c r="DW179" t="s">
         <v>1805</v>
-      </c>
-      <c r="DV179">
-        <v>2</v>
-      </c>
-      <c r="DW179" t="s">
-        <v>1806</v>
       </c>
       <c r="EJ179">
         <v>6</v>
@@ -50862,7 +50865,7 @@
         <v>1</v>
       </c>
       <c r="FM179" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="FP179">
         <v>25</v>
@@ -50910,7 +50913,7 @@
         <v>-2</v>
       </c>
       <c r="GH179" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="GI179">
         <v>-2</v>
@@ -50928,10 +50931,10 @@
         <v>800</v>
       </c>
       <c r="GO179" t="s">
+        <v>1808</v>
+      </c>
+      <c r="GP179" t="s">
         <v>1809</v>
-      </c>
-      <c r="GP179" t="s">
-        <v>1810</v>
       </c>
       <c r="GQ179" t="s">
         <v>665</v>
@@ -50943,7 +50946,7 @@
         <v>-9</v>
       </c>
       <c r="GV179" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="GW179">
         <v>0</v>
@@ -51012,7 +51015,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="180" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>896</v>
       </c>
@@ -51053,7 +51056,7 @@
         <v>1</v>
       </c>
       <c r="FL180" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="FP180">
         <v>25</v>
@@ -51119,7 +51122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="181" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>898</v>
       </c>
@@ -51160,37 +51163,37 @@
         <v>2</v>
       </c>
       <c r="AQ181" t="s">
+        <v>1812</v>
+      </c>
+      <c r="AV181" t="s">
         <v>1813</v>
       </c>
-      <c r="AV181" t="s">
+      <c r="BO181">
+        <v>2</v>
+      </c>
+      <c r="BP181">
+        <v>2</v>
+      </c>
+      <c r="BQ181">
+        <v>1</v>
+      </c>
+      <c r="BR181">
+        <v>1</v>
+      </c>
+      <c r="BS181">
+        <v>1</v>
+      </c>
+      <c r="BT181">
+        <v>2</v>
+      </c>
+      <c r="BU181">
+        <v>1</v>
+      </c>
+      <c r="BV181">
+        <v>1</v>
+      </c>
+      <c r="CJ181" t="s">
         <v>1814</v>
-      </c>
-      <c r="BO181">
-        <v>2</v>
-      </c>
-      <c r="BP181">
-        <v>2</v>
-      </c>
-      <c r="BQ181">
-        <v>1</v>
-      </c>
-      <c r="BR181">
-        <v>1</v>
-      </c>
-      <c r="BS181">
-        <v>1</v>
-      </c>
-      <c r="BT181">
-        <v>2</v>
-      </c>
-      <c r="BU181">
-        <v>1</v>
-      </c>
-      <c r="BV181">
-        <v>1</v>
-      </c>
-      <c r="CJ181" t="s">
-        <v>1815</v>
       </c>
       <c r="CU181">
         <v>120</v>
@@ -51217,7 +51220,7 @@
         <v>1</v>
       </c>
       <c r="DX181" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="EA181" t="s">
         <v>641</v>
@@ -51244,13 +51247,13 @@
         <v>2</v>
       </c>
       <c r="EI181" t="s">
+        <v>1816</v>
+      </c>
+      <c r="FK181">
+        <v>2</v>
+      </c>
+      <c r="FL181" t="s">
         <v>1817</v>
-      </c>
-      <c r="FK181">
-        <v>2</v>
-      </c>
-      <c r="FL181" t="s">
-        <v>1818</v>
       </c>
       <c r="FP181">
         <v>25</v>
@@ -51298,7 +51301,7 @@
         <v>20</v>
       </c>
       <c r="GH181" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="GI181">
         <v>5</v>
@@ -51319,10 +51322,10 @@
         <v>800</v>
       </c>
       <c r="GO181" t="s">
+        <v>1818</v>
+      </c>
+      <c r="GP181" t="s">
         <v>1819</v>
-      </c>
-      <c r="GP181" t="s">
-        <v>1820</v>
       </c>
       <c r="GQ181" t="s">
         <v>603</v>
@@ -51334,7 +51337,7 @@
         <v>-9</v>
       </c>
       <c r="GV181" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="GW181">
         <v>0</v>
@@ -51403,7 +51406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="182" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>900</v>
       </c>
@@ -51444,7 +51447,7 @@
         <v>1</v>
       </c>
       <c r="AT182" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="AW182" t="s">
         <v>641</v>
@@ -51474,7 +51477,7 @@
         <v>2</v>
       </c>
       <c r="CH182" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="DM182" t="s">
         <v>628</v>
@@ -51501,37 +51504,37 @@
         <v>1</v>
       </c>
       <c r="DZ182" t="s">
+        <v>1823</v>
+      </c>
+      <c r="ES182">
+        <v>2</v>
+      </c>
+      <c r="ET182">
+        <v>2</v>
+      </c>
+      <c r="EU182">
+        <v>2</v>
+      </c>
+      <c r="EV182">
+        <v>1</v>
+      </c>
+      <c r="EW182">
+        <v>1</v>
+      </c>
+      <c r="EX182">
+        <v>2</v>
+      </c>
+      <c r="EY182">
+        <v>1</v>
+      </c>
+      <c r="EZ182">
+        <v>2</v>
+      </c>
+      <c r="FA182" t="s">
         <v>1824</v>
       </c>
-      <c r="ES182">
-        <v>2</v>
-      </c>
-      <c r="ET182">
-        <v>2</v>
-      </c>
-      <c r="EU182">
-        <v>2</v>
-      </c>
-      <c r="EV182">
-        <v>1</v>
-      </c>
-      <c r="EW182">
-        <v>1</v>
-      </c>
-      <c r="EX182">
-        <v>2</v>
-      </c>
-      <c r="EY182">
-        <v>1</v>
-      </c>
-      <c r="EZ182">
-        <v>2</v>
-      </c>
-      <c r="FA182" t="s">
+      <c r="FN182" t="s">
         <v>1825</v>
-      </c>
-      <c r="FN182" t="s">
-        <v>1826</v>
       </c>
       <c r="FP182">
         <v>25</v>
@@ -51579,7 +51582,7 @@
         <v>15</v>
       </c>
       <c r="GH182" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="GI182">
         <v>5</v>
@@ -51600,10 +51603,10 @@
         <v>800</v>
       </c>
       <c r="GO182" t="s">
+        <v>1826</v>
+      </c>
+      <c r="GP182" t="s">
         <v>1827</v>
-      </c>
-      <c r="GP182" t="s">
-        <v>1828</v>
       </c>
       <c r="GQ182" t="s">
         <v>603</v>
@@ -51681,7 +51684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>902</v>
       </c>
@@ -51725,7 +51728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>904</v>
       </c>
@@ -51769,7 +51772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>907</v>
       </c>
@@ -51786,40 +51789,40 @@
         <v>44193.913402777776</v>
       </c>
       <c r="CL185" t="s">
+        <v>1828</v>
+      </c>
+      <c r="CM185">
+        <v>2</v>
+      </c>
+      <c r="CN185">
+        <v>1</v>
+      </c>
+      <c r="CO185">
+        <v>1</v>
+      </c>
+      <c r="CP185">
+        <v>1</v>
+      </c>
+      <c r="CQ185">
+        <v>1</v>
+      </c>
+      <c r="CR185">
+        <v>1</v>
+      </c>
+      <c r="CS185">
+        <v>2</v>
+      </c>
+      <c r="CT185" t="s">
         <v>1829</v>
       </c>
-      <c r="CM185">
-        <v>2</v>
-      </c>
-      <c r="CN185">
-        <v>1</v>
-      </c>
-      <c r="CO185">
-        <v>1</v>
-      </c>
-      <c r="CP185">
-        <v>1</v>
-      </c>
-      <c r="CQ185">
-        <v>1</v>
-      </c>
-      <c r="CR185">
-        <v>1</v>
-      </c>
-      <c r="CS185">
-        <v>2</v>
-      </c>
-      <c r="CT185" t="s">
+      <c r="DW185" t="s">
         <v>1830</v>
       </c>
-      <c r="DW185" t="s">
+      <c r="EJ185" t="s">
         <v>1831</v>
       </c>
-      <c r="EJ185" t="s">
+      <c r="FM185" t="s">
         <v>1832</v>
-      </c>
-      <c r="FM185" t="s">
-        <v>1833</v>
       </c>
       <c r="FP185">
         <v>26</v>
@@ -51888,7 +51891,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="186" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>908</v>
       </c>
@@ -51932,7 +51935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>910</v>
       </c>
@@ -51976,7 +51979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>911</v>
       </c>
@@ -52020,7 +52023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>913</v>
       </c>
@@ -52094,7 +52097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>915</v>
       </c>
@@ -52111,7 +52114,7 @@
         <v>44194.046307870369</v>
       </c>
       <c r="CH190" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="FP190">
         <v>26</v>
@@ -52174,7 +52177,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>916</v>
       </c>
@@ -52245,7 +52248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>917</v>
       </c>
@@ -52289,7 +52292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:445" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:445" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>923</v>
       </c>

</xml_diff>

<commit_message>
added preparation for aoi analysis
</commit_message>
<xml_diff>
--- a/REyeker-DataAnalyses-Python/Book4.xlsx
+++ b/REyeker-DataAnalyses-Python/Book4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\REyeker\REyeker-DataAnalyses-Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DC09AF-6DFB-47B1-82C8-098F2748BBE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376DAC6C-9FC2-4937-ADC9-48C1795126A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5010" yWindow="2850" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5634,9 +5634,6 @@
     <t xml:space="preserve">62-17 62-58 340-65 498-65 119-99 256-91 485-103 95-101 96-141 291-131 183-169 431-163 238-112 578-164 121-241 364-231 171-294 470-313 311-353 278-417 199-344 111-256 69-25 77-104 222-74 565-68 89-97 336-110 643-102 85-126 326-129 104-126 122-159 365-164 593-158 242-119 163-258 479-240 182-299 258-342 324-388 309-427 338-361 314-396 287-442 310-168 166-104 161-140 402-160 359-340 267-429 295-385 275-414 114-493 49-548 210-421 299-353 174-247 448-242 149-273 344-303 344-303 126-328 433-337 229-385 224-418 319-308 306-360 354-389 339-413 381-346 361-381 319-113 473-107 221-149 350-89 554-106 </t>
   </si>
   <si>
-    <t xml:space="preserve">244-51 541-84 236-98 458-112 -1-104 178-106 283-129 514-141 214-159 425-145 278-271 368-245 346-117 286-145 300-234 511-242 257-283 281-310 357-333 590-333 857-324 344-334 342-271 380-315 637-333 875-326 500-341 801-329 464-94 238-127 482-118 337-219 319-268 274-292 285-321 507-321 544-242 293-238 557-240 345-297 505-331 727-316 599-361 592-333 836-331 573-324 282-301 310-237 667-231 473-130 278-123 191-69 322-95 493-125 510-68 228-69 594-350 605-329 796-326 625-233 157-228 435-237 600-248 719-253 584-327 787-329 556-334 342-319 705-336 378-281 627-323 820-336 595-338 313-115 242-281 478-241 549-328 434-149 292-133 628-329 847-327 335-115 401-100 </t>
-  </si>
-  <si>
     <t xml:space="preserve">156-8 229-66 535-70 236-114 526-140 315-122 281-204 254-250 259-276 299-282 486-303 276-272 389-306 242-250 367-304 636-301 537-301 301-287 248-266 246-206 249-235 255-286 236-307 230-230 219-248 291-273 269-222 </t>
   </si>
   <si>
@@ -5989,6 +5986,9 @@
   </si>
   <si>
     <t xml:space="preserve">168-44 325-19 260-51 88-47 409-45 551-67 275-82 133-82 130-107 128-121 120-167 128-200 385-187 59-227 122-258 245-271 57-314 180-287 172-272 200-264 177-228 188-101 166-38 146-91 201-98 147-200 145-248 172-282 209-282 165-210 179-266 223-202 230-267 142-234 155-281 180-271 252-1 173-69 255-278 86-7 212-77 206-277 199-89 216-274 209-206 163-250 198-274 146-112 137-62 97-87 106-92 166-202 400-182 216-240 100-220 138-248 135-275 192-271 115-274 160-272 236-207 293-125 422-184 138-200 159-231 169-255 170-12 188-84 233-218 207-235 209-131 167-95 205-79 200-237 153-295 157-280 307-325 399-311 322-306 177-279 178-238 247-195 223-256 258-275 351-327 315-296 175-257 129-272 205-266 165-214 423-177 211-225 81-221 136-241 138-208 137-257 126-229 137-210 122-217 132-265 161-294 171-275 205-242 209-268 176-207 176-225 176-225 180-205 276-194 489-210 158-235 126-275 131-272 162-82 173-266 180-121 182-98 181-80 189-287 148-258 168-89 166-255 173-279 168-280 169-265 163-275 177-309 199-275 267-224 278-277 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">244-51 541-84 236-98 458-112 1-104 178-106 283-129 514-141 214-159 425-145 278-271 368-245 346-117 286-145 300-234 511-242 257-283 281-310 357-333 590-333 857-324 344-334 342-271 380-315 637-333 875-326 500-341 801-329 464-94 238-127 482-118 337-219 319-268 274-292 285-321 507-321 544-242 293-238 557-240 345-297 505-331 727-316 599-361 592-333 836-331 573-324 282-301 310-237 667-231 473-130 278-123 191-69 322-95 493-125 510-68 228-69 594-350 605-329 796-326 625-233 157-228 435-237 600-248 719-253 584-327 787-329 556-334 342-319 705-336 378-281 627-323 820-336 595-338 313-115 242-281 478-241 549-328 434-149 292-133 628-329 847-327 335-115 401-100 </t>
   </si>
 </sst>
 </file>
@@ -6315,8 +6315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:QC193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="IA138" workbookViewId="0">
-      <selection activeCell="IG152" sqref="IG152"/>
+    <sheetView tabSelected="1" topLeftCell="AU154" workbookViewId="0">
+      <selection activeCell="AV165" sqref="AV165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44052,7 +44052,7 @@
         <v>1</v>
       </c>
       <c r="IG149" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="IH149" t="s">
         <v>1632</v>
@@ -47333,7 +47333,7 @@
         <v>1</v>
       </c>
       <c r="AV165" t="s">
-        <v>1716</v>
+        <v>1834</v>
       </c>
       <c r="BO165">
         <v>3</v>
@@ -47360,7 +47360,7 @@
         <v>1</v>
       </c>
       <c r="CJ165" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="CU165">
         <v>120</v>
@@ -47387,7 +47387,7 @@
         <v>1</v>
       </c>
       <c r="DX165" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="EA165">
         <v>31623426175536</v>
@@ -47417,7 +47417,7 @@
         <v>1</v>
       </c>
       <c r="FL165" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="FP165">
         <v>23</v>
@@ -47465,7 +47465,7 @@
         <v>-2</v>
       </c>
       <c r="GH165" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="GI165">
         <v>-2</v>
@@ -47483,10 +47483,10 @@
         <v>800</v>
       </c>
       <c r="GO165" t="s">
+        <v>1720</v>
+      </c>
+      <c r="GP165" t="s">
         <v>1721</v>
-      </c>
-      <c r="GP165" t="s">
-        <v>1722</v>
       </c>
       <c r="GQ165" t="s">
         <v>665</v>
@@ -47498,7 +47498,7 @@
         <v>-9</v>
       </c>
       <c r="GV165" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="GW165">
         <v>0</v>
@@ -47594,16 +47594,16 @@
         <v>1</v>
       </c>
       <c r="MV165" t="s">
+        <v>1723</v>
+      </c>
+      <c r="MW165" t="s">
         <v>1724</v>
       </c>
-      <c r="MW165" t="s">
+      <c r="MX165" t="s">
         <v>1725</v>
       </c>
-      <c r="MX165" t="s">
+      <c r="MY165" t="s">
         <v>1726</v>
-      </c>
-      <c r="MY165" t="s">
-        <v>1727</v>
       </c>
       <c r="MZ165">
         <v>3</v>
@@ -48104,7 +48104,7 @@
         <v>2</v>
       </c>
       <c r="AS168" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="BF168">
         <v>6</v>
@@ -48131,34 +48131,34 @@
         <v>1</v>
       </c>
       <c r="CI168" t="s">
+        <v>1728</v>
+      </c>
+      <c r="DD168">
+        <v>1</v>
+      </c>
+      <c r="DE168">
+        <v>2</v>
+      </c>
+      <c r="DF168">
+        <v>1</v>
+      </c>
+      <c r="DG168">
+        <v>1</v>
+      </c>
+      <c r="DH168">
+        <v>2</v>
+      </c>
+      <c r="DI168">
+        <v>1</v>
+      </c>
+      <c r="DJ168">
+        <v>1</v>
+      </c>
+      <c r="DK168">
+        <v>1</v>
+      </c>
+      <c r="DY168" t="s">
         <v>1729</v>
-      </c>
-      <c r="DD168">
-        <v>1</v>
-      </c>
-      <c r="DE168">
-        <v>2</v>
-      </c>
-      <c r="DF168">
-        <v>1</v>
-      </c>
-      <c r="DG168">
-        <v>1</v>
-      </c>
-      <c r="DH168">
-        <v>2</v>
-      </c>
-      <c r="DI168">
-        <v>1</v>
-      </c>
-      <c r="DJ168">
-        <v>1</v>
-      </c>
-      <c r="DK168">
-        <v>1</v>
-      </c>
-      <c r="DY168" t="s">
-        <v>1730</v>
       </c>
       <c r="FB168">
         <v>11</v>
@@ -48185,7 +48185,7 @@
         <v>1</v>
       </c>
       <c r="FO168" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="FP168">
         <v>23</v>
@@ -48233,7 +48233,7 @@
         <v>-2</v>
       </c>
       <c r="GH168" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="GI168">
         <v>-2</v>
@@ -48251,10 +48251,10 @@
         <v>800</v>
       </c>
       <c r="GO168" t="s">
+        <v>1732</v>
+      </c>
+      <c r="GP168" t="s">
         <v>1733</v>
-      </c>
-      <c r="GP168" t="s">
-        <v>1734</v>
       </c>
       <c r="GQ168" t="s">
         <v>938</v>
@@ -48376,7 +48376,7 @@
         <v>1</v>
       </c>
       <c r="AS169" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="BF169">
         <v>6</v>
@@ -48403,34 +48403,34 @@
         <v>1</v>
       </c>
       <c r="CI169" t="s">
+        <v>1735</v>
+      </c>
+      <c r="DD169">
+        <v>2</v>
+      </c>
+      <c r="DE169">
+        <v>1</v>
+      </c>
+      <c r="DF169">
+        <v>1</v>
+      </c>
+      <c r="DG169">
+        <v>1</v>
+      </c>
+      <c r="DH169">
+        <v>1</v>
+      </c>
+      <c r="DI169">
+        <v>2</v>
+      </c>
+      <c r="DJ169">
+        <v>1</v>
+      </c>
+      <c r="DK169">
+        <v>1</v>
+      </c>
+      <c r="DY169" t="s">
         <v>1736</v>
-      </c>
-      <c r="DD169">
-        <v>2</v>
-      </c>
-      <c r="DE169">
-        <v>1</v>
-      </c>
-      <c r="DF169">
-        <v>1</v>
-      </c>
-      <c r="DG169">
-        <v>1</v>
-      </c>
-      <c r="DH169">
-        <v>1</v>
-      </c>
-      <c r="DI169">
-        <v>2</v>
-      </c>
-      <c r="DJ169">
-        <v>1</v>
-      </c>
-      <c r="DK169">
-        <v>1</v>
-      </c>
-      <c r="DY169" t="s">
-        <v>1737</v>
       </c>
       <c r="FB169" t="s">
         <v>628</v>
@@ -48457,10 +48457,10 @@
         <v>2</v>
       </c>
       <c r="FJ169" t="s">
+        <v>1737</v>
+      </c>
+      <c r="FO169" t="s">
         <v>1738</v>
-      </c>
-      <c r="FO169" t="s">
-        <v>1739</v>
       </c>
       <c r="FP169">
         <v>23</v>
@@ -48517,7 +48517,7 @@
         <v>1</v>
       </c>
       <c r="II169" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="MZ169">
         <v>115</v>
@@ -48600,31 +48600,31 @@
         <v>44185.565428240741</v>
       </c>
       <c r="H170" t="s">
+        <v>1740</v>
+      </c>
+      <c r="I170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <v>1</v>
+      </c>
+      <c r="K170">
+        <v>2</v>
+      </c>
+      <c r="L170">
+        <v>1</v>
+      </c>
+      <c r="M170">
+        <v>1</v>
+      </c>
+      <c r="N170">
+        <v>1</v>
+      </c>
+      <c r="O170">
+        <v>1</v>
+      </c>
+      <c r="AS170" t="s">
         <v>1741</v>
-      </c>
-      <c r="I170">
-        <v>1</v>
-      </c>
-      <c r="J170">
-        <v>1</v>
-      </c>
-      <c r="K170">
-        <v>2</v>
-      </c>
-      <c r="L170">
-        <v>1</v>
-      </c>
-      <c r="M170">
-        <v>1</v>
-      </c>
-      <c r="N170">
-        <v>1</v>
-      </c>
-      <c r="O170">
-        <v>1</v>
-      </c>
-      <c r="AS170" t="s">
-        <v>1742</v>
       </c>
       <c r="BF170">
         <v>6</v>
@@ -48651,7 +48651,7 @@
         <v>1</v>
       </c>
       <c r="CI170" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="FP170">
         <v>23</v>
@@ -48767,7 +48767,7 @@
         <v>1</v>
       </c>
       <c r="AS171" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="BF171">
         <v>6</v>
@@ -48794,34 +48794,34 @@
         <v>1</v>
       </c>
       <c r="CI171" t="s">
+        <v>1744</v>
+      </c>
+      <c r="DD171">
+        <v>2</v>
+      </c>
+      <c r="DE171">
+        <v>2</v>
+      </c>
+      <c r="DF171">
+        <v>1</v>
+      </c>
+      <c r="DG171">
+        <v>1</v>
+      </c>
+      <c r="DH171">
+        <v>2</v>
+      </c>
+      <c r="DI171">
+        <v>1</v>
+      </c>
+      <c r="DJ171">
+        <v>1</v>
+      </c>
+      <c r="DK171">
+        <v>1</v>
+      </c>
+      <c r="DY171" t="s">
         <v>1745</v>
-      </c>
-      <c r="DD171">
-        <v>2</v>
-      </c>
-      <c r="DE171">
-        <v>2</v>
-      </c>
-      <c r="DF171">
-        <v>1</v>
-      </c>
-      <c r="DG171">
-        <v>1</v>
-      </c>
-      <c r="DH171">
-        <v>2</v>
-      </c>
-      <c r="DI171">
-        <v>1</v>
-      </c>
-      <c r="DJ171">
-        <v>1</v>
-      </c>
-      <c r="DK171">
-        <v>1</v>
-      </c>
-      <c r="DY171" t="s">
-        <v>1746</v>
       </c>
       <c r="FB171" t="s">
         <v>628</v>
@@ -48848,7 +48848,7 @@
         <v>1</v>
       </c>
       <c r="FO171" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="FP171">
         <v>24</v>
@@ -48896,7 +48896,7 @@
         <v>-2</v>
       </c>
       <c r="GH171" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="GI171">
         <v>-2</v>
@@ -48917,7 +48917,7 @@
         <v>77180254195</v>
       </c>
       <c r="GP171" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="GQ171" t="s">
         <v>938</v>
@@ -48929,7 +48929,7 @@
         <v>2</v>
       </c>
       <c r="GU171" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="GW171">
         <v>1</v>
@@ -48959,7 +48959,7 @@
         <v>1</v>
       </c>
       <c r="HG171" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="HH171">
         <v>2</v>
@@ -49007,10 +49007,10 @@
         <v>2</v>
       </c>
       <c r="HW171" t="s">
+        <v>1751</v>
+      </c>
+      <c r="HX171" t="s">
         <v>1752</v>
-      </c>
-      <c r="HX171" t="s">
-        <v>1753</v>
       </c>
       <c r="HY171">
         <v>4</v>
@@ -49034,16 +49034,16 @@
         <v>1</v>
       </c>
       <c r="IG171" t="s">
+        <v>1753</v>
+      </c>
+      <c r="IH171" t="s">
         <v>1754</v>
       </c>
-      <c r="IH171" t="s">
+      <c r="II171" t="s">
         <v>1755</v>
       </c>
-      <c r="II171" t="s">
+      <c r="IJ171" t="s">
         <v>1756</v>
-      </c>
-      <c r="IJ171" t="s">
-        <v>1757</v>
       </c>
       <c r="MZ171">
         <v>1</v>
@@ -49150,37 +49150,37 @@
         <v>44185.596226851849</v>
       </c>
       <c r="AI172" t="s">
+        <v>1757</v>
+      </c>
+      <c r="AJ172">
+        <v>2</v>
+      </c>
+      <c r="AK172">
+        <v>2</v>
+      </c>
+      <c r="AL172">
+        <v>1</v>
+      </c>
+      <c r="AM172">
+        <v>1</v>
+      </c>
+      <c r="AN172">
+        <v>1</v>
+      </c>
+      <c r="AO172">
+        <v>2</v>
+      </c>
+      <c r="AP172">
+        <v>2</v>
+      </c>
+      <c r="AQ172" t="s">
         <v>1758</v>
       </c>
-      <c r="AJ172">
-        <v>2</v>
-      </c>
-      <c r="AK172">
-        <v>2</v>
-      </c>
-      <c r="AL172">
-        <v>1</v>
-      </c>
-      <c r="AM172">
-        <v>1</v>
-      </c>
-      <c r="AN172">
-        <v>1</v>
-      </c>
-      <c r="AO172">
-        <v>2</v>
-      </c>
-      <c r="AP172">
-        <v>2</v>
-      </c>
-      <c r="AQ172" t="s">
+      <c r="AV172" t="s">
         <v>1759</v>
       </c>
-      <c r="AV172" t="s">
+      <c r="BO172" t="s">
         <v>1760</v>
-      </c>
-      <c r="BO172" t="s">
-        <v>1761</v>
       </c>
       <c r="BP172">
         <v>3</v>
@@ -49204,10 +49204,10 @@
         <v>2</v>
       </c>
       <c r="BW172" t="s">
+        <v>1761</v>
+      </c>
+      <c r="CJ172" t="s">
         <v>1762</v>
-      </c>
-      <c r="CJ172" t="s">
-        <v>1763</v>
       </c>
       <c r="CU172">
         <v>120</v>
@@ -49234,7 +49234,7 @@
         <v>1</v>
       </c>
       <c r="DX172" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="EA172" t="s">
         <v>641</v>
@@ -49264,7 +49264,7 @@
         <v>1</v>
       </c>
       <c r="FL172" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="FP172">
         <v>24</v>
@@ -49312,7 +49312,7 @@
         <v>20</v>
       </c>
       <c r="GH172" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="GI172">
         <v>5</v>
@@ -49333,10 +49333,10 @@
         <v>800</v>
       </c>
       <c r="GO172" t="s">
+        <v>1766</v>
+      </c>
+      <c r="GP172" t="s">
         <v>1767</v>
-      </c>
-      <c r="GP172" t="s">
-        <v>1768</v>
       </c>
       <c r="GQ172" t="s">
         <v>603</v>
@@ -49348,91 +49348,91 @@
         <v>2</v>
       </c>
       <c r="GU172" t="s">
+        <v>1768</v>
+      </c>
+      <c r="GV172" t="s">
         <v>1769</v>
       </c>
-      <c r="GV172" t="s">
+      <c r="GW172">
+        <v>1</v>
+      </c>
+      <c r="LM172" t="s">
         <v>1770</v>
       </c>
-      <c r="GW172">
-        <v>1</v>
-      </c>
-      <c r="LM172" t="s">
+      <c r="LN172">
+        <v>1</v>
+      </c>
+      <c r="LO172">
+        <v>1</v>
+      </c>
+      <c r="LP172">
+        <v>1</v>
+      </c>
+      <c r="LQ172">
+        <v>1</v>
+      </c>
+      <c r="LR172">
+        <v>1</v>
+      </c>
+      <c r="LS172">
+        <v>1</v>
+      </c>
+      <c r="LT172">
+        <v>2</v>
+      </c>
+      <c r="LU172" t="s">
         <v>1771</v>
       </c>
-      <c r="LN172">
-        <v>1</v>
-      </c>
-      <c r="LO172">
-        <v>1</v>
-      </c>
-      <c r="LP172">
-        <v>1</v>
-      </c>
-      <c r="LQ172">
-        <v>1</v>
-      </c>
-      <c r="LR172">
-        <v>1</v>
-      </c>
-      <c r="LS172">
-        <v>1</v>
-      </c>
-      <c r="LT172">
-        <v>2</v>
-      </c>
-      <c r="LU172" t="s">
+      <c r="LV172" t="s">
         <v>1772</v>
       </c>
-      <c r="LV172" t="s">
+      <c r="LW172">
+        <v>1</v>
+      </c>
+      <c r="LX172">
+        <v>1</v>
+      </c>
+      <c r="LY172">
+        <v>2</v>
+      </c>
+      <c r="LZ172">
+        <v>1</v>
+      </c>
+      <c r="MA172">
+        <v>1</v>
+      </c>
+      <c r="MB172">
+        <v>1</v>
+      </c>
+      <c r="MC172">
+        <v>1</v>
+      </c>
+      <c r="ME172" t="s">
         <v>1773</v>
       </c>
-      <c r="LW172">
-        <v>1</v>
-      </c>
-      <c r="LX172">
-        <v>1</v>
-      </c>
-      <c r="LY172">
-        <v>2</v>
-      </c>
-      <c r="LZ172">
-        <v>1</v>
-      </c>
-      <c r="MA172">
-        <v>1</v>
-      </c>
-      <c r="MB172">
-        <v>1</v>
-      </c>
-      <c r="MC172">
-        <v>1</v>
-      </c>
-      <c r="ME172" t="s">
+      <c r="MF172">
+        <v>1</v>
+      </c>
+      <c r="MG172">
+        <v>1</v>
+      </c>
+      <c r="MH172">
+        <v>2</v>
+      </c>
+      <c r="MI172">
+        <v>1</v>
+      </c>
+      <c r="MJ172">
+        <v>1</v>
+      </c>
+      <c r="MK172">
+        <v>1</v>
+      </c>
+      <c r="ML172">
+        <v>1</v>
+      </c>
+      <c r="MN172" t="s">
         <v>1774</v>
-      </c>
-      <c r="MF172">
-        <v>1</v>
-      </c>
-      <c r="MG172">
-        <v>1</v>
-      </c>
-      <c r="MH172">
-        <v>2</v>
-      </c>
-      <c r="MI172">
-        <v>1</v>
-      </c>
-      <c r="MJ172">
-        <v>1</v>
-      </c>
-      <c r="MK172">
-        <v>1</v>
-      </c>
-      <c r="ML172">
-        <v>1</v>
-      </c>
-      <c r="MN172" t="s">
-        <v>1775</v>
       </c>
       <c r="MO172">
         <v>4</v>
@@ -49456,16 +49456,16 @@
         <v>1</v>
       </c>
       <c r="MV172" t="s">
+        <v>1775</v>
+      </c>
+      <c r="MW172" t="s">
         <v>1776</v>
       </c>
-      <c r="MW172" t="s">
+      <c r="MX172" t="s">
         <v>1777</v>
       </c>
-      <c r="MX172" t="s">
+      <c r="MY172" t="s">
         <v>1778</v>
-      </c>
-      <c r="MY172" t="s">
-        <v>1779</v>
       </c>
       <c r="MZ172">
         <v>29</v>
@@ -49596,7 +49596,7 @@
         <v>1</v>
       </c>
       <c r="AU173" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="BX173" t="s">
         <v>636</v>
@@ -49623,7 +49623,7 @@
         <v>1</v>
       </c>
       <c r="CK173" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="CL173" t="s">
         <v>641</v>
@@ -49653,7 +49653,7 @@
         <v>2</v>
       </c>
       <c r="DW173" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="EJ173">
         <v>6</v>
@@ -49680,7 +49680,7 @@
         <v>1</v>
       </c>
       <c r="FM173" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="FP173">
         <v>24</v>
@@ -49728,7 +49728,7 @@
         <v>-2</v>
       </c>
       <c r="GH173" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="GI173">
         <v>-2</v>
@@ -49746,10 +49746,10 @@
         <v>800</v>
       </c>
       <c r="GO173" t="s">
+        <v>1784</v>
+      </c>
+      <c r="GP173" t="s">
         <v>1785</v>
-      </c>
-      <c r="GP173" t="s">
-        <v>1786</v>
       </c>
       <c r="GQ173" t="s">
         <v>665</v>
@@ -49761,7 +49761,7 @@
         <v>1</v>
       </c>
       <c r="GV173" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="GW173">
         <v>0</v>
@@ -49922,7 +49922,7 @@
         <v>1</v>
       </c>
       <c r="DZ174" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="ES174">
         <v>2</v>
@@ -50012,10 +50012,10 @@
         <v>355</v>
       </c>
       <c r="GO174" t="s">
+        <v>1788</v>
+      </c>
+      <c r="GP174" t="s">
         <v>1789</v>
-      </c>
-      <c r="GP174" t="s">
-        <v>1790</v>
       </c>
       <c r="GQ174" t="s">
         <v>938</v>
@@ -50027,7 +50027,7 @@
         <v>-9</v>
       </c>
       <c r="GV174" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="GW174">
         <v>1</v>
@@ -50285,7 +50285,7 @@
         <v>1</v>
       </c>
       <c r="AT177" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="AW177">
         <v>61</v>
@@ -50315,7 +50315,7 @@
         <v>1</v>
       </c>
       <c r="CH177" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="DM177" t="s">
         <v>628</v>
@@ -50342,34 +50342,34 @@
         <v>1</v>
       </c>
       <c r="DZ177" t="s">
+        <v>1793</v>
+      </c>
+      <c r="ES177">
+        <v>2</v>
+      </c>
+      <c r="ET177">
+        <v>1</v>
+      </c>
+      <c r="EU177">
+        <v>1</v>
+      </c>
+      <c r="EV177">
+        <v>2</v>
+      </c>
+      <c r="EW177">
+        <v>1</v>
+      </c>
+      <c r="EX177">
+        <v>1</v>
+      </c>
+      <c r="EY177">
+        <v>1</v>
+      </c>
+      <c r="EZ177">
+        <v>1</v>
+      </c>
+      <c r="FN177" t="s">
         <v>1794</v>
-      </c>
-      <c r="ES177">
-        <v>2</v>
-      </c>
-      <c r="ET177">
-        <v>1</v>
-      </c>
-      <c r="EU177">
-        <v>1</v>
-      </c>
-      <c r="EV177">
-        <v>2</v>
-      </c>
-      <c r="EW177">
-        <v>1</v>
-      </c>
-      <c r="EX177">
-        <v>1</v>
-      </c>
-      <c r="EY177">
-        <v>1</v>
-      </c>
-      <c r="EZ177">
-        <v>1</v>
-      </c>
-      <c r="FN177" t="s">
-        <v>1795</v>
       </c>
       <c r="FP177">
         <v>25</v>
@@ -50500,7 +50500,7 @@
         <v>2</v>
       </c>
       <c r="AS178" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="BF178">
         <v>6</v>
@@ -50527,34 +50527,34 @@
         <v>1</v>
       </c>
       <c r="CI178" t="s">
+        <v>1796</v>
+      </c>
+      <c r="DD178">
+        <v>2</v>
+      </c>
+      <c r="DE178">
+        <v>1</v>
+      </c>
+      <c r="DF178">
+        <v>1</v>
+      </c>
+      <c r="DG178">
+        <v>2</v>
+      </c>
+      <c r="DH178">
+        <v>1</v>
+      </c>
+      <c r="DI178">
+        <v>1</v>
+      </c>
+      <c r="DJ178">
+        <v>1</v>
+      </c>
+      <c r="DK178">
+        <v>1</v>
+      </c>
+      <c r="DY178" t="s">
         <v>1797</v>
-      </c>
-      <c r="DD178">
-        <v>2</v>
-      </c>
-      <c r="DE178">
-        <v>1</v>
-      </c>
-      <c r="DF178">
-        <v>1</v>
-      </c>
-      <c r="DG178">
-        <v>2</v>
-      </c>
-      <c r="DH178">
-        <v>1</v>
-      </c>
-      <c r="DI178">
-        <v>1</v>
-      </c>
-      <c r="DJ178">
-        <v>1</v>
-      </c>
-      <c r="DK178">
-        <v>1</v>
-      </c>
-      <c r="DY178" t="s">
-        <v>1798</v>
       </c>
       <c r="FB178" t="s">
         <v>628</v>
@@ -50581,7 +50581,7 @@
         <v>1</v>
       </c>
       <c r="FO178" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="FP178">
         <v>25</v>
@@ -50665,7 +50665,7 @@
         <v>-9</v>
       </c>
       <c r="GV178" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="GW178">
         <v>1</v>
@@ -50775,7 +50775,7 @@
         <v>1</v>
       </c>
       <c r="AU179" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="BX179" t="s">
         <v>636</v>
@@ -50802,10 +50802,10 @@
         <v>2</v>
       </c>
       <c r="CF179" t="s">
+        <v>1801</v>
+      </c>
+      <c r="CK179" t="s">
         <v>1802</v>
-      </c>
-      <c r="CK179" t="s">
-        <v>1803</v>
       </c>
       <c r="CL179" t="s">
         <v>641</v>
@@ -50832,13 +50832,13 @@
         <v>2</v>
       </c>
       <c r="CT179" t="s">
+        <v>1803</v>
+      </c>
+      <c r="DV179">
+        <v>2</v>
+      </c>
+      <c r="DW179" t="s">
         <v>1804</v>
-      </c>
-      <c r="DV179">
-        <v>2</v>
-      </c>
-      <c r="DW179" t="s">
-        <v>1805</v>
       </c>
       <c r="EJ179">
         <v>6</v>
@@ -50865,7 +50865,7 @@
         <v>1</v>
       </c>
       <c r="FM179" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="FP179">
         <v>25</v>
@@ -50913,7 +50913,7 @@
         <v>-2</v>
       </c>
       <c r="GH179" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="GI179">
         <v>-2</v>
@@ -50931,10 +50931,10 @@
         <v>800</v>
       </c>
       <c r="GO179" t="s">
+        <v>1807</v>
+      </c>
+      <c r="GP179" t="s">
         <v>1808</v>
-      </c>
-      <c r="GP179" t="s">
-        <v>1809</v>
       </c>
       <c r="GQ179" t="s">
         <v>665</v>
@@ -50946,7 +50946,7 @@
         <v>-9</v>
       </c>
       <c r="GV179" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="GW179">
         <v>0</v>
@@ -51056,7 +51056,7 @@
         <v>1</v>
       </c>
       <c r="FL180" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="FP180">
         <v>25</v>
@@ -51163,37 +51163,37 @@
         <v>2</v>
       </c>
       <c r="AQ181" t="s">
+        <v>1811</v>
+      </c>
+      <c r="AV181" t="s">
         <v>1812</v>
       </c>
-      <c r="AV181" t="s">
+      <c r="BO181">
+        <v>2</v>
+      </c>
+      <c r="BP181">
+        <v>2</v>
+      </c>
+      <c r="BQ181">
+        <v>1</v>
+      </c>
+      <c r="BR181">
+        <v>1</v>
+      </c>
+      <c r="BS181">
+        <v>1</v>
+      </c>
+      <c r="BT181">
+        <v>2</v>
+      </c>
+      <c r="BU181">
+        <v>1</v>
+      </c>
+      <c r="BV181">
+        <v>1</v>
+      </c>
+      <c r="CJ181" t="s">
         <v>1813</v>
-      </c>
-      <c r="BO181">
-        <v>2</v>
-      </c>
-      <c r="BP181">
-        <v>2</v>
-      </c>
-      <c r="BQ181">
-        <v>1</v>
-      </c>
-      <c r="BR181">
-        <v>1</v>
-      </c>
-      <c r="BS181">
-        <v>1</v>
-      </c>
-      <c r="BT181">
-        <v>2</v>
-      </c>
-      <c r="BU181">
-        <v>1</v>
-      </c>
-      <c r="BV181">
-        <v>1</v>
-      </c>
-      <c r="CJ181" t="s">
-        <v>1814</v>
       </c>
       <c r="CU181">
         <v>120</v>
@@ -51220,7 +51220,7 @@
         <v>1</v>
       </c>
       <c r="DX181" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="EA181" t="s">
         <v>641</v>
@@ -51247,13 +51247,13 @@
         <v>2</v>
       </c>
       <c r="EI181" t="s">
+        <v>1815</v>
+      </c>
+      <c r="FK181">
+        <v>2</v>
+      </c>
+      <c r="FL181" t="s">
         <v>1816</v>
-      </c>
-      <c r="FK181">
-        <v>2</v>
-      </c>
-      <c r="FL181" t="s">
-        <v>1817</v>
       </c>
       <c r="FP181">
         <v>25</v>
@@ -51301,7 +51301,7 @@
         <v>20</v>
       </c>
       <c r="GH181" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="GI181">
         <v>5</v>
@@ -51322,10 +51322,10 @@
         <v>800</v>
       </c>
       <c r="GO181" t="s">
+        <v>1817</v>
+      </c>
+      <c r="GP181" t="s">
         <v>1818</v>
-      </c>
-      <c r="GP181" t="s">
-        <v>1819</v>
       </c>
       <c r="GQ181" t="s">
         <v>603</v>
@@ -51337,7 +51337,7 @@
         <v>-9</v>
       </c>
       <c r="GV181" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="GW181">
         <v>0</v>
@@ -51447,7 +51447,7 @@
         <v>1</v>
       </c>
       <c r="AT182" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="AW182" t="s">
         <v>641</v>
@@ -51477,7 +51477,7 @@
         <v>2</v>
       </c>
       <c r="CH182" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="DM182" t="s">
         <v>628</v>
@@ -51504,37 +51504,37 @@
         <v>1</v>
       </c>
       <c r="DZ182" t="s">
+        <v>1822</v>
+      </c>
+      <c r="ES182">
+        <v>2</v>
+      </c>
+      <c r="ET182">
+        <v>2</v>
+      </c>
+      <c r="EU182">
+        <v>2</v>
+      </c>
+      <c r="EV182">
+        <v>1</v>
+      </c>
+      <c r="EW182">
+        <v>1</v>
+      </c>
+      <c r="EX182">
+        <v>2</v>
+      </c>
+      <c r="EY182">
+        <v>1</v>
+      </c>
+      <c r="EZ182">
+        <v>2</v>
+      </c>
+      <c r="FA182" t="s">
         <v>1823</v>
       </c>
-      <c r="ES182">
-        <v>2</v>
-      </c>
-      <c r="ET182">
-        <v>2</v>
-      </c>
-      <c r="EU182">
-        <v>2</v>
-      </c>
-      <c r="EV182">
-        <v>1</v>
-      </c>
-      <c r="EW182">
-        <v>1</v>
-      </c>
-      <c r="EX182">
-        <v>2</v>
-      </c>
-      <c r="EY182">
-        <v>1</v>
-      </c>
-      <c r="EZ182">
-        <v>2</v>
-      </c>
-      <c r="FA182" t="s">
+      <c r="FN182" t="s">
         <v>1824</v>
-      </c>
-      <c r="FN182" t="s">
-        <v>1825</v>
       </c>
       <c r="FP182">
         <v>25</v>
@@ -51603,10 +51603,10 @@
         <v>800</v>
       </c>
       <c r="GO182" t="s">
+        <v>1825</v>
+      </c>
+      <c r="GP182" t="s">
         <v>1826</v>
-      </c>
-      <c r="GP182" t="s">
-        <v>1827</v>
       </c>
       <c r="GQ182" t="s">
         <v>603</v>
@@ -51789,40 +51789,40 @@
         <v>44193.913402777776</v>
       </c>
       <c r="CL185" t="s">
+        <v>1827</v>
+      </c>
+      <c r="CM185">
+        <v>2</v>
+      </c>
+      <c r="CN185">
+        <v>1</v>
+      </c>
+      <c r="CO185">
+        <v>1</v>
+      </c>
+      <c r="CP185">
+        <v>1</v>
+      </c>
+      <c r="CQ185">
+        <v>1</v>
+      </c>
+      <c r="CR185">
+        <v>1</v>
+      </c>
+      <c r="CS185">
+        <v>2</v>
+      </c>
+      <c r="CT185" t="s">
         <v>1828</v>
       </c>
-      <c r="CM185">
-        <v>2</v>
-      </c>
-      <c r="CN185">
-        <v>1</v>
-      </c>
-      <c r="CO185">
-        <v>1</v>
-      </c>
-      <c r="CP185">
-        <v>1</v>
-      </c>
-      <c r="CQ185">
-        <v>1</v>
-      </c>
-      <c r="CR185">
-        <v>1</v>
-      </c>
-      <c r="CS185">
-        <v>2</v>
-      </c>
-      <c r="CT185" t="s">
+      <c r="DW185" t="s">
         <v>1829</v>
       </c>
-      <c r="DW185" t="s">
+      <c r="EJ185" t="s">
         <v>1830</v>
       </c>
-      <c r="EJ185" t="s">
+      <c r="FM185" t="s">
         <v>1831</v>
-      </c>
-      <c r="FM185" t="s">
-        <v>1832</v>
       </c>
       <c r="FP185">
         <v>26</v>
@@ -52114,7 +52114,7 @@
         <v>44194.046307870369</v>
       </c>
       <c r="CH190" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="FP190">
         <v>26</v>

</xml_diff>